<commit_message>
DB Schema Updated : UAPIMI Methodology
</commit_message>
<xml_diff>
--- a/Database Schema Proteen.xlsx
+++ b/Database Schema Proteen.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="540" windowWidth="20490" windowHeight="7215"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="20490" windowHeight="7155"/>
   </bookViews>
   <sheets>
     <sheet name="Schema" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2813" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2863" uniqueCount="309">
   <si>
     <t>No</t>
   </si>
@@ -928,6 +928,21 @@
   </si>
   <si>
     <t>1 - Normal , 2 - Youtube, 3 - Vimeo</t>
+  </si>
+  <si>
+    <t>pro_bits_baskets_interest_type_scale</t>
+  </si>
+  <si>
+    <t>bits_basket</t>
+  </si>
+  <si>
+    <t>bits_interest_type</t>
+  </si>
+  <si>
+    <t>bits_scale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 - High, 2 - Moderate, 3 - Low </t>
   </si>
 </sst>
 </file>
@@ -1162,7 +1177,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="115">
+  <cellXfs count="118">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1460,6 +1475,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1808,10 +1832,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K462"/>
+  <dimension ref="A1:K472"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A352" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K361" sqref="K361"/>
+    <sheetView tabSelected="1" topLeftCell="A460" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I472" sqref="I472"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1831,49 +1855,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="108" t="s">
+      <c r="A1" s="111" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="108"/>
-      <c r="C1" s="108"/>
-      <c r="D1" s="108"/>
-      <c r="E1" s="108"/>
-      <c r="F1" s="108"/>
-      <c r="G1" s="108"/>
-      <c r="H1" s="108"/>
-      <c r="I1" s="108"/>
-      <c r="J1" s="108"/>
-      <c r="K1" s="108"/>
+      <c r="B1" s="111"/>
+      <c r="C1" s="111"/>
+      <c r="D1" s="111"/>
+      <c r="E1" s="111"/>
+      <c r="F1" s="111"/>
+      <c r="G1" s="111"/>
+      <c r="H1" s="111"/>
+      <c r="I1" s="111"/>
+      <c r="J1" s="111"/>
+      <c r="K1" s="111"/>
     </row>
     <row r="2" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="109" t="s">
+      <c r="A2" s="112" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="110"/>
-      <c r="C2" s="110"/>
-      <c r="D2" s="110"/>
-      <c r="E2" s="110"/>
-      <c r="F2" s="110"/>
-      <c r="G2" s="110"/>
-      <c r="H2" s="110"/>
-      <c r="I2" s="110"/>
-      <c r="J2" s="110"/>
-      <c r="K2" s="111"/>
+      <c r="B2" s="113"/>
+      <c r="C2" s="113"/>
+      <c r="D2" s="113"/>
+      <c r="E2" s="113"/>
+      <c r="F2" s="113"/>
+      <c r="G2" s="113"/>
+      <c r="H2" s="113"/>
+      <c r="I2" s="113"/>
+      <c r="J2" s="113"/>
+      <c r="K2" s="114"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="104" t="s">
+      <c r="A3" s="107" t="s">
         <v>156</v>
       </c>
-      <c r="B3" s="105"/>
-      <c r="C3" s="105"/>
-      <c r="D3" s="105"/>
-      <c r="E3" s="105"/>
-      <c r="F3" s="105"/>
-      <c r="G3" s="105"/>
-      <c r="H3" s="105"/>
-      <c r="I3" s="105"/>
-      <c r="J3" s="105"/>
-      <c r="K3" s="106"/>
+      <c r="B3" s="108"/>
+      <c r="C3" s="108"/>
+      <c r="D3" s="108"/>
+      <c r="E3" s="108"/>
+      <c r="F3" s="108"/>
+      <c r="G3" s="108"/>
+      <c r="H3" s="108"/>
+      <c r="I3" s="108"/>
+      <c r="J3" s="108"/>
+      <c r="K3" s="109"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
@@ -2066,7 +2090,7 @@
         <v>1</v>
       </c>
       <c r="F10" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10" s="13"/>
       <c r="H10" s="13" t="s">
@@ -2079,45 +2103,45 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="102"/>
-      <c r="B11" s="102"/>
-      <c r="C11" s="102"/>
-      <c r="D11" s="102"/>
-      <c r="E11" s="102"/>
-      <c r="F11" s="102"/>
-      <c r="G11" s="102"/>
-      <c r="H11" s="102"/>
-      <c r="I11" s="102"/>
-      <c r="J11" s="102"/>
-      <c r="K11" s="102"/>
+      <c r="A11" s="105"/>
+      <c r="B11" s="105"/>
+      <c r="C11" s="105"/>
+      <c r="D11" s="105"/>
+      <c r="E11" s="105"/>
+      <c r="F11" s="105"/>
+      <c r="G11" s="105"/>
+      <c r="H11" s="105"/>
+      <c r="I11" s="105"/>
+      <c r="J11" s="105"/>
+      <c r="K11" s="105"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="103"/>
-      <c r="B12" s="103"/>
-      <c r="C12" s="103"/>
-      <c r="D12" s="103"/>
-      <c r="E12" s="103"/>
-      <c r="F12" s="103"/>
-      <c r="G12" s="103"/>
-      <c r="H12" s="103"/>
-      <c r="I12" s="103"/>
-      <c r="J12" s="103"/>
-      <c r="K12" s="103"/>
+      <c r="A12" s="106"/>
+      <c r="B12" s="106"/>
+      <c r="C12" s="106"/>
+      <c r="D12" s="106"/>
+      <c r="E12" s="106"/>
+      <c r="F12" s="106"/>
+      <c r="G12" s="106"/>
+      <c r="H12" s="106"/>
+      <c r="I12" s="106"/>
+      <c r="J12" s="106"/>
+      <c r="K12" s="106"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="112" t="s">
+      <c r="A13" s="115" t="s">
         <v>156</v>
       </c>
-      <c r="B13" s="113"/>
-      <c r="C13" s="113"/>
-      <c r="D13" s="113"/>
-      <c r="E13" s="113"/>
-      <c r="F13" s="113"/>
-      <c r="G13" s="113"/>
-      <c r="H13" s="113"/>
-      <c r="I13" s="113"/>
-      <c r="J13" s="113"/>
-      <c r="K13" s="114"/>
+      <c r="B13" s="116"/>
+      <c r="C13" s="116"/>
+      <c r="D13" s="116"/>
+      <c r="E13" s="116"/>
+      <c r="F13" s="116"/>
+      <c r="G13" s="116"/>
+      <c r="H13" s="116"/>
+      <c r="I13" s="116"/>
+      <c r="J13" s="116"/>
+      <c r="K13" s="117"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="66" t="s">
@@ -2309,8 +2333,8 @@
       <c r="E20" s="80">
         <v>1</v>
       </c>
-      <c r="F20" s="79">
-        <v>0</v>
+      <c r="F20" s="13">
+        <v>1</v>
       </c>
       <c r="G20" s="79"/>
       <c r="H20" s="79" t="s">
@@ -2323,45 +2347,45 @@
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="107"/>
-      <c r="B21" s="107"/>
-      <c r="C21" s="107"/>
-      <c r="D21" s="107"/>
-      <c r="E21" s="107"/>
-      <c r="F21" s="107"/>
-      <c r="G21" s="107"/>
-      <c r="H21" s="107"/>
-      <c r="I21" s="107"/>
-      <c r="J21" s="107"/>
-      <c r="K21" s="107"/>
+      <c r="A21" s="110"/>
+      <c r="B21" s="110"/>
+      <c r="C21" s="110"/>
+      <c r="D21" s="110"/>
+      <c r="E21" s="110"/>
+      <c r="F21" s="110"/>
+      <c r="G21" s="110"/>
+      <c r="H21" s="110"/>
+      <c r="I21" s="110"/>
+      <c r="J21" s="110"/>
+      <c r="K21" s="110"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="103"/>
-      <c r="B22" s="103"/>
-      <c r="C22" s="103"/>
-      <c r="D22" s="103"/>
-      <c r="E22" s="103"/>
-      <c r="F22" s="103"/>
-      <c r="G22" s="103"/>
-      <c r="H22" s="103"/>
-      <c r="I22" s="103"/>
-      <c r="J22" s="103"/>
-      <c r="K22" s="103"/>
+      <c r="A22" s="106"/>
+      <c r="B22" s="106"/>
+      <c r="C22" s="106"/>
+      <c r="D22" s="106"/>
+      <c r="E22" s="106"/>
+      <c r="F22" s="106"/>
+      <c r="G22" s="106"/>
+      <c r="H22" s="106"/>
+      <c r="I22" s="106"/>
+      <c r="J22" s="106"/>
+      <c r="K22" s="106"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="104" t="s">
+      <c r="A23" s="107" t="s">
         <v>144</v>
       </c>
-      <c r="B23" s="105"/>
-      <c r="C23" s="105"/>
-      <c r="D23" s="105"/>
-      <c r="E23" s="105"/>
-      <c r="F23" s="105"/>
-      <c r="G23" s="105"/>
-      <c r="H23" s="105"/>
-      <c r="I23" s="105"/>
-      <c r="J23" s="105"/>
-      <c r="K23" s="106"/>
+      <c r="B23" s="108"/>
+      <c r="C23" s="108"/>
+      <c r="D23" s="108"/>
+      <c r="E23" s="108"/>
+      <c r="F23" s="108"/>
+      <c r="G23" s="108"/>
+      <c r="H23" s="108"/>
+      <c r="I23" s="108"/>
+      <c r="J23" s="108"/>
+      <c r="K23" s="109"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="20" t="s">
@@ -2581,7 +2605,7 @@
         <v>1</v>
       </c>
       <c r="F31" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G31" s="13"/>
       <c r="H31" s="13" t="s">
@@ -2594,45 +2618,45 @@
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="102"/>
-      <c r="B32" s="102"/>
-      <c r="C32" s="102"/>
-      <c r="D32" s="102"/>
-      <c r="E32" s="102"/>
-      <c r="F32" s="102"/>
-      <c r="G32" s="102"/>
-      <c r="H32" s="102"/>
-      <c r="I32" s="102"/>
-      <c r="J32" s="102"/>
-      <c r="K32" s="102"/>
+      <c r="A32" s="105"/>
+      <c r="B32" s="105"/>
+      <c r="C32" s="105"/>
+      <c r="D32" s="105"/>
+      <c r="E32" s="105"/>
+      <c r="F32" s="105"/>
+      <c r="G32" s="105"/>
+      <c r="H32" s="105"/>
+      <c r="I32" s="105"/>
+      <c r="J32" s="105"/>
+      <c r="K32" s="105"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="103"/>
-      <c r="B33" s="103"/>
-      <c r="C33" s="103"/>
-      <c r="D33" s="103"/>
-      <c r="E33" s="103"/>
-      <c r="F33" s="103"/>
-      <c r="G33" s="103"/>
-      <c r="H33" s="103"/>
-      <c r="I33" s="103"/>
-      <c r="J33" s="103"/>
-      <c r="K33" s="103"/>
+      <c r="A33" s="106"/>
+      <c r="B33" s="106"/>
+      <c r="C33" s="106"/>
+      <c r="D33" s="106"/>
+      <c r="E33" s="106"/>
+      <c r="F33" s="106"/>
+      <c r="G33" s="106"/>
+      <c r="H33" s="106"/>
+      <c r="I33" s="106"/>
+      <c r="J33" s="106"/>
+      <c r="K33" s="106"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="104" t="s">
+      <c r="A34" s="107" t="s">
         <v>30</v>
       </c>
-      <c r="B34" s="105"/>
-      <c r="C34" s="105"/>
-      <c r="D34" s="105"/>
-      <c r="E34" s="105"/>
-      <c r="F34" s="105"/>
-      <c r="G34" s="105"/>
-      <c r="H34" s="105"/>
-      <c r="I34" s="105"/>
-      <c r="J34" s="105"/>
-      <c r="K34" s="106"/>
+      <c r="B34" s="108"/>
+      <c r="C34" s="108"/>
+      <c r="D34" s="108"/>
+      <c r="E34" s="108"/>
+      <c r="F34" s="108"/>
+      <c r="G34" s="108"/>
+      <c r="H34" s="108"/>
+      <c r="I34" s="108"/>
+      <c r="J34" s="108"/>
+      <c r="K34" s="109"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="20" t="s">
@@ -3460,7 +3484,7 @@
         <v>1</v>
       </c>
       <c r="F64" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G64" s="13"/>
       <c r="H64" s="13" t="s">
@@ -3473,45 +3497,45 @@
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A65" s="102"/>
-      <c r="B65" s="102"/>
-      <c r="C65" s="102"/>
-      <c r="D65" s="102"/>
-      <c r="E65" s="102"/>
-      <c r="F65" s="102"/>
-      <c r="G65" s="102"/>
-      <c r="H65" s="102"/>
-      <c r="I65" s="102"/>
-      <c r="J65" s="102"/>
-      <c r="K65" s="102"/>
+      <c r="A65" s="105"/>
+      <c r="B65" s="105"/>
+      <c r="C65" s="105"/>
+      <c r="D65" s="105"/>
+      <c r="E65" s="105"/>
+      <c r="F65" s="105"/>
+      <c r="G65" s="105"/>
+      <c r="H65" s="105"/>
+      <c r="I65" s="105"/>
+      <c r="J65" s="105"/>
+      <c r="K65" s="105"/>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A66" s="103"/>
-      <c r="B66" s="103"/>
-      <c r="C66" s="103"/>
-      <c r="D66" s="103"/>
-      <c r="E66" s="103"/>
-      <c r="F66" s="103"/>
-      <c r="G66" s="103"/>
-      <c r="H66" s="103"/>
-      <c r="I66" s="103"/>
-      <c r="J66" s="103"/>
-      <c r="K66" s="103"/>
+      <c r="A66" s="106"/>
+      <c r="B66" s="106"/>
+      <c r="C66" s="106"/>
+      <c r="D66" s="106"/>
+      <c r="E66" s="106"/>
+      <c r="F66" s="106"/>
+      <c r="G66" s="106"/>
+      <c r="H66" s="106"/>
+      <c r="I66" s="106"/>
+      <c r="J66" s="106"/>
+      <c r="K66" s="106"/>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A67" s="104" t="s">
+      <c r="A67" s="107" t="s">
         <v>295</v>
       </c>
-      <c r="B67" s="105"/>
-      <c r="C67" s="105"/>
-      <c r="D67" s="105"/>
-      <c r="E67" s="105"/>
-      <c r="F67" s="105"/>
-      <c r="G67" s="105"/>
-      <c r="H67" s="105"/>
-      <c r="I67" s="105"/>
-      <c r="J67" s="105"/>
-      <c r="K67" s="106"/>
+      <c r="B67" s="108"/>
+      <c r="C67" s="108"/>
+      <c r="D67" s="108"/>
+      <c r="E67" s="108"/>
+      <c r="F67" s="108"/>
+      <c r="G67" s="108"/>
+      <c r="H67" s="108"/>
+      <c r="I67" s="108"/>
+      <c r="J67" s="108"/>
+      <c r="K67" s="109"/>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="20" t="s">
@@ -3752,45 +3776,45 @@
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A76" s="102"/>
-      <c r="B76" s="102"/>
-      <c r="C76" s="102"/>
-      <c r="D76" s="102"/>
-      <c r="E76" s="102"/>
-      <c r="F76" s="102"/>
-      <c r="G76" s="102"/>
-      <c r="H76" s="102"/>
-      <c r="I76" s="102"/>
-      <c r="J76" s="102"/>
-      <c r="K76" s="102"/>
+      <c r="A76" s="105"/>
+      <c r="B76" s="105"/>
+      <c r="C76" s="105"/>
+      <c r="D76" s="105"/>
+      <c r="E76" s="105"/>
+      <c r="F76" s="105"/>
+      <c r="G76" s="105"/>
+      <c r="H76" s="105"/>
+      <c r="I76" s="105"/>
+      <c r="J76" s="105"/>
+      <c r="K76" s="105"/>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A77" s="103"/>
-      <c r="B77" s="103"/>
-      <c r="C77" s="103"/>
-      <c r="D77" s="103"/>
-      <c r="E77" s="103"/>
-      <c r="F77" s="103"/>
-      <c r="G77" s="103"/>
-      <c r="H77" s="103"/>
-      <c r="I77" s="103"/>
-      <c r="J77" s="103"/>
-      <c r="K77" s="103"/>
+      <c r="A77" s="106"/>
+      <c r="B77" s="106"/>
+      <c r="C77" s="106"/>
+      <c r="D77" s="106"/>
+      <c r="E77" s="106"/>
+      <c r="F77" s="106"/>
+      <c r="G77" s="106"/>
+      <c r="H77" s="106"/>
+      <c r="I77" s="106"/>
+      <c r="J77" s="106"/>
+      <c r="K77" s="106"/>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A78" s="104" t="s">
+      <c r="A78" s="107" t="s">
         <v>251</v>
       </c>
-      <c r="B78" s="105"/>
-      <c r="C78" s="105"/>
-      <c r="D78" s="105"/>
-      <c r="E78" s="105"/>
-      <c r="F78" s="105"/>
-      <c r="G78" s="105"/>
-      <c r="H78" s="105"/>
-      <c r="I78" s="105"/>
-      <c r="J78" s="105"/>
-      <c r="K78" s="106"/>
+      <c r="B78" s="108"/>
+      <c r="C78" s="108"/>
+      <c r="D78" s="108"/>
+      <c r="E78" s="108"/>
+      <c r="F78" s="108"/>
+      <c r="G78" s="108"/>
+      <c r="H78" s="108"/>
+      <c r="I78" s="108"/>
+      <c r="J78" s="108"/>
+      <c r="K78" s="109"/>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="20" t="s">
@@ -3991,7 +4015,7 @@
         <v>1</v>
       </c>
       <c r="F85" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G85" s="13"/>
       <c r="H85" s="13" t="s">
@@ -4004,45 +4028,45 @@
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A86" s="107"/>
-      <c r="B86" s="107"/>
-      <c r="C86" s="107"/>
-      <c r="D86" s="107"/>
-      <c r="E86" s="107"/>
-      <c r="F86" s="107"/>
-      <c r="G86" s="107"/>
-      <c r="H86" s="107"/>
-      <c r="I86" s="107"/>
-      <c r="J86" s="107"/>
-      <c r="K86" s="107"/>
+      <c r="A86" s="110"/>
+      <c r="B86" s="110"/>
+      <c r="C86" s="110"/>
+      <c r="D86" s="110"/>
+      <c r="E86" s="110"/>
+      <c r="F86" s="110"/>
+      <c r="G86" s="110"/>
+      <c r="H86" s="110"/>
+      <c r="I86" s="110"/>
+      <c r="J86" s="110"/>
+      <c r="K86" s="110"/>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A87" s="103"/>
-      <c r="B87" s="103"/>
-      <c r="C87" s="103"/>
-      <c r="D87" s="103"/>
-      <c r="E87" s="103"/>
-      <c r="F87" s="103"/>
-      <c r="G87" s="103"/>
-      <c r="H87" s="103"/>
-      <c r="I87" s="103"/>
-      <c r="J87" s="103"/>
-      <c r="K87" s="103"/>
+      <c r="A87" s="106"/>
+      <c r="B87" s="106"/>
+      <c r="C87" s="106"/>
+      <c r="D87" s="106"/>
+      <c r="E87" s="106"/>
+      <c r="F87" s="106"/>
+      <c r="G87" s="106"/>
+      <c r="H87" s="106"/>
+      <c r="I87" s="106"/>
+      <c r="J87" s="106"/>
+      <c r="K87" s="106"/>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A88" s="104" t="s">
+      <c r="A88" s="107" t="s">
         <v>147</v>
       </c>
-      <c r="B88" s="105"/>
-      <c r="C88" s="105"/>
-      <c r="D88" s="105"/>
-      <c r="E88" s="105"/>
-      <c r="F88" s="105"/>
-      <c r="G88" s="105"/>
-      <c r="H88" s="105"/>
-      <c r="I88" s="105"/>
-      <c r="J88" s="105"/>
-      <c r="K88" s="106"/>
+      <c r="B88" s="108"/>
+      <c r="C88" s="108"/>
+      <c r="D88" s="108"/>
+      <c r="E88" s="108"/>
+      <c r="F88" s="108"/>
+      <c r="G88" s="108"/>
+      <c r="H88" s="108"/>
+      <c r="I88" s="108"/>
+      <c r="J88" s="108"/>
+      <c r="K88" s="109"/>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
@@ -4318,7 +4342,7 @@
         <v>1</v>
       </c>
       <c r="F98" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G98" s="13"/>
       <c r="H98" s="13" t="s">
@@ -4331,45 +4355,45 @@
       </c>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A99" s="107"/>
-      <c r="B99" s="107"/>
-      <c r="C99" s="107"/>
-      <c r="D99" s="107"/>
-      <c r="E99" s="107"/>
-      <c r="F99" s="107"/>
-      <c r="G99" s="107"/>
-      <c r="H99" s="107"/>
-      <c r="I99" s="107"/>
-      <c r="J99" s="107"/>
-      <c r="K99" s="107"/>
+      <c r="A99" s="110"/>
+      <c r="B99" s="110"/>
+      <c r="C99" s="110"/>
+      <c r="D99" s="110"/>
+      <c r="E99" s="110"/>
+      <c r="F99" s="110"/>
+      <c r="G99" s="110"/>
+      <c r="H99" s="110"/>
+      <c r="I99" s="110"/>
+      <c r="J99" s="110"/>
+      <c r="K99" s="110"/>
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A100" s="103"/>
-      <c r="B100" s="103"/>
-      <c r="C100" s="103"/>
-      <c r="D100" s="103"/>
-      <c r="E100" s="103"/>
-      <c r="F100" s="103"/>
-      <c r="G100" s="103"/>
-      <c r="H100" s="103"/>
-      <c r="I100" s="103"/>
-      <c r="J100" s="103"/>
-      <c r="K100" s="103"/>
+      <c r="A100" s="106"/>
+      <c r="B100" s="106"/>
+      <c r="C100" s="106"/>
+      <c r="D100" s="106"/>
+      <c r="E100" s="106"/>
+      <c r="F100" s="106"/>
+      <c r="G100" s="106"/>
+      <c r="H100" s="106"/>
+      <c r="I100" s="106"/>
+      <c r="J100" s="106"/>
+      <c r="K100" s="106"/>
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A101" s="104" t="s">
+      <c r="A101" s="107" t="s">
         <v>291</v>
       </c>
-      <c r="B101" s="105"/>
-      <c r="C101" s="105"/>
-      <c r="D101" s="105"/>
-      <c r="E101" s="105"/>
-      <c r="F101" s="105"/>
-      <c r="G101" s="105"/>
-      <c r="H101" s="105"/>
-      <c r="I101" s="105"/>
-      <c r="J101" s="105"/>
-      <c r="K101" s="106"/>
+      <c r="B101" s="108"/>
+      <c r="C101" s="108"/>
+      <c r="D101" s="108"/>
+      <c r="E101" s="108"/>
+      <c r="F101" s="108"/>
+      <c r="G101" s="108"/>
+      <c r="H101" s="108"/>
+      <c r="I101" s="108"/>
+      <c r="J101" s="108"/>
+      <c r="K101" s="109"/>
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
@@ -4597,7 +4621,7 @@
         <v>1</v>
       </c>
       <c r="F109" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G109" s="13"/>
       <c r="H109" s="13" t="s">
@@ -4610,45 +4634,45 @@
       </c>
     </row>
     <row r="110" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A110" s="102"/>
-      <c r="B110" s="102"/>
-      <c r="C110" s="102"/>
-      <c r="D110" s="102"/>
-      <c r="E110" s="102"/>
-      <c r="F110" s="102"/>
-      <c r="G110" s="102"/>
-      <c r="H110" s="102"/>
-      <c r="I110" s="102"/>
-      <c r="J110" s="102"/>
-      <c r="K110" s="102"/>
+      <c r="A110" s="105"/>
+      <c r="B110" s="105"/>
+      <c r="C110" s="105"/>
+      <c r="D110" s="105"/>
+      <c r="E110" s="105"/>
+      <c r="F110" s="105"/>
+      <c r="G110" s="105"/>
+      <c r="H110" s="105"/>
+      <c r="I110" s="105"/>
+      <c r="J110" s="105"/>
+      <c r="K110" s="105"/>
     </row>
     <row r="111" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A111" s="103"/>
-      <c r="B111" s="103"/>
-      <c r="C111" s="103"/>
-      <c r="D111" s="103"/>
-      <c r="E111" s="103"/>
-      <c r="F111" s="103"/>
-      <c r="G111" s="103"/>
-      <c r="H111" s="103"/>
-      <c r="I111" s="103"/>
-      <c r="J111" s="103"/>
-      <c r="K111" s="103"/>
+      <c r="A111" s="106"/>
+      <c r="B111" s="106"/>
+      <c r="C111" s="106"/>
+      <c r="D111" s="106"/>
+      <c r="E111" s="106"/>
+      <c r="F111" s="106"/>
+      <c r="G111" s="106"/>
+      <c r="H111" s="106"/>
+      <c r="I111" s="106"/>
+      <c r="J111" s="106"/>
+      <c r="K111" s="106"/>
     </row>
     <row r="112" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A112" s="104" t="s">
+      <c r="A112" s="107" t="s">
         <v>43</v>
       </c>
-      <c r="B112" s="105"/>
-      <c r="C112" s="105"/>
-      <c r="D112" s="105"/>
-      <c r="E112" s="105"/>
-      <c r="F112" s="105"/>
-      <c r="G112" s="105"/>
-      <c r="H112" s="105"/>
-      <c r="I112" s="105"/>
-      <c r="J112" s="105"/>
-      <c r="K112" s="106"/>
+      <c r="B112" s="108"/>
+      <c r="C112" s="108"/>
+      <c r="D112" s="108"/>
+      <c r="E112" s="108"/>
+      <c r="F112" s="108"/>
+      <c r="G112" s="108"/>
+      <c r="H112" s="108"/>
+      <c r="I112" s="108"/>
+      <c r="J112" s="108"/>
+      <c r="K112" s="109"/>
     </row>
     <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113" s="20" t="s">
@@ -4963,7 +4987,7 @@
         <v>1</v>
       </c>
       <c r="F123" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G123" s="13"/>
       <c r="H123" s="13" t="s">
@@ -4976,45 +5000,45 @@
       </c>
     </row>
     <row r="124" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A124" s="102"/>
-      <c r="B124" s="102"/>
-      <c r="C124" s="102"/>
-      <c r="D124" s="102"/>
-      <c r="E124" s="102"/>
-      <c r="F124" s="102"/>
-      <c r="G124" s="102"/>
-      <c r="H124" s="102"/>
-      <c r="I124" s="102"/>
-      <c r="J124" s="102"/>
-      <c r="K124" s="102"/>
+      <c r="A124" s="105"/>
+      <c r="B124" s="105"/>
+      <c r="C124" s="105"/>
+      <c r="D124" s="105"/>
+      <c r="E124" s="105"/>
+      <c r="F124" s="105"/>
+      <c r="G124" s="105"/>
+      <c r="H124" s="105"/>
+      <c r="I124" s="105"/>
+      <c r="J124" s="105"/>
+      <c r="K124" s="105"/>
     </row>
     <row r="125" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A125" s="103"/>
-      <c r="B125" s="103"/>
-      <c r="C125" s="103"/>
-      <c r="D125" s="103"/>
-      <c r="E125" s="103"/>
-      <c r="F125" s="103"/>
-      <c r="G125" s="103"/>
-      <c r="H125" s="103"/>
-      <c r="I125" s="103"/>
-      <c r="J125" s="103"/>
-      <c r="K125" s="103"/>
+      <c r="A125" s="106"/>
+      <c r="B125" s="106"/>
+      <c r="C125" s="106"/>
+      <c r="D125" s="106"/>
+      <c r="E125" s="106"/>
+      <c r="F125" s="106"/>
+      <c r="G125" s="106"/>
+      <c r="H125" s="106"/>
+      <c r="I125" s="106"/>
+      <c r="J125" s="106"/>
+      <c r="K125" s="106"/>
     </row>
     <row r="126" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A126" s="104" t="s">
+      <c r="A126" s="107" t="s">
         <v>50</v>
       </c>
-      <c r="B126" s="105"/>
-      <c r="C126" s="105"/>
-      <c r="D126" s="105"/>
-      <c r="E126" s="105"/>
-      <c r="F126" s="105"/>
-      <c r="G126" s="105"/>
-      <c r="H126" s="105"/>
-      <c r="I126" s="105"/>
-      <c r="J126" s="105"/>
-      <c r="K126" s="106"/>
+      <c r="B126" s="108"/>
+      <c r="C126" s="108"/>
+      <c r="D126" s="108"/>
+      <c r="E126" s="108"/>
+      <c r="F126" s="108"/>
+      <c r="G126" s="108"/>
+      <c r="H126" s="108"/>
+      <c r="I126" s="108"/>
+      <c r="J126" s="108"/>
+      <c r="K126" s="109"/>
     </row>
     <row r="127" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A127" s="20" t="s">
@@ -5348,7 +5372,7 @@
         <v>1</v>
       </c>
       <c r="F138" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G138" s="13"/>
       <c r="H138" s="13" t="s">
@@ -5361,45 +5385,45 @@
       </c>
     </row>
     <row r="139" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A139" s="102"/>
-      <c r="B139" s="102"/>
-      <c r="C139" s="102"/>
-      <c r="D139" s="102"/>
-      <c r="E139" s="102"/>
-      <c r="F139" s="102"/>
-      <c r="G139" s="102"/>
-      <c r="H139" s="102"/>
-      <c r="I139" s="102"/>
-      <c r="J139" s="102"/>
-      <c r="K139" s="102"/>
+      <c r="A139" s="105"/>
+      <c r="B139" s="105"/>
+      <c r="C139" s="105"/>
+      <c r="D139" s="105"/>
+      <c r="E139" s="105"/>
+      <c r="F139" s="105"/>
+      <c r="G139" s="105"/>
+      <c r="H139" s="105"/>
+      <c r="I139" s="105"/>
+      <c r="J139" s="105"/>
+      <c r="K139" s="105"/>
     </row>
     <row r="140" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A140" s="103"/>
-      <c r="B140" s="103"/>
-      <c r="C140" s="103"/>
-      <c r="D140" s="103"/>
-      <c r="E140" s="103"/>
-      <c r="F140" s="103"/>
-      <c r="G140" s="103"/>
-      <c r="H140" s="103"/>
-      <c r="I140" s="103"/>
-      <c r="J140" s="103"/>
-      <c r="K140" s="103"/>
+      <c r="A140" s="106"/>
+      <c r="B140" s="106"/>
+      <c r="C140" s="106"/>
+      <c r="D140" s="106"/>
+      <c r="E140" s="106"/>
+      <c r="F140" s="106"/>
+      <c r="G140" s="106"/>
+      <c r="H140" s="106"/>
+      <c r="I140" s="106"/>
+      <c r="J140" s="106"/>
+      <c r="K140" s="106"/>
     </row>
     <row r="141" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A141" s="104" t="s">
+      <c r="A141" s="107" t="s">
         <v>49</v>
       </c>
-      <c r="B141" s="105"/>
-      <c r="C141" s="105"/>
-      <c r="D141" s="105"/>
-      <c r="E141" s="105"/>
-      <c r="F141" s="105"/>
-      <c r="G141" s="105"/>
-      <c r="H141" s="105"/>
-      <c r="I141" s="105"/>
-      <c r="J141" s="105"/>
-      <c r="K141" s="106"/>
+      <c r="B141" s="108"/>
+      <c r="C141" s="108"/>
+      <c r="D141" s="108"/>
+      <c r="E141" s="108"/>
+      <c r="F141" s="108"/>
+      <c r="G141" s="108"/>
+      <c r="H141" s="108"/>
+      <c r="I141" s="108"/>
+      <c r="J141" s="108"/>
+      <c r="K141" s="109"/>
     </row>
     <row r="142" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A142" s="20" t="s">
@@ -5799,7 +5823,7 @@
         <v>1</v>
       </c>
       <c r="F155" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G155" s="13"/>
       <c r="H155" s="13" t="s">
@@ -5812,45 +5836,45 @@
       </c>
     </row>
     <row r="156" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A156" s="102"/>
-      <c r="B156" s="102"/>
-      <c r="C156" s="102"/>
-      <c r="D156" s="102"/>
-      <c r="E156" s="102"/>
-      <c r="F156" s="102"/>
-      <c r="G156" s="102"/>
-      <c r="H156" s="102"/>
-      <c r="I156" s="102"/>
-      <c r="J156" s="102"/>
-      <c r="K156" s="102"/>
+      <c r="A156" s="105"/>
+      <c r="B156" s="105"/>
+      <c r="C156" s="105"/>
+      <c r="D156" s="105"/>
+      <c r="E156" s="105"/>
+      <c r="F156" s="105"/>
+      <c r="G156" s="105"/>
+      <c r="H156" s="105"/>
+      <c r="I156" s="105"/>
+      <c r="J156" s="105"/>
+      <c r="K156" s="105"/>
     </row>
     <row r="157" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A157" s="103"/>
-      <c r="B157" s="103"/>
-      <c r="C157" s="103"/>
-      <c r="D157" s="103"/>
-      <c r="E157" s="103"/>
-      <c r="F157" s="103"/>
-      <c r="G157" s="103"/>
-      <c r="H157" s="103"/>
-      <c r="I157" s="103"/>
-      <c r="J157" s="103"/>
-      <c r="K157" s="103"/>
+      <c r="A157" s="106"/>
+      <c r="B157" s="106"/>
+      <c r="C157" s="106"/>
+      <c r="D157" s="106"/>
+      <c r="E157" s="106"/>
+      <c r="F157" s="106"/>
+      <c r="G157" s="106"/>
+      <c r="H157" s="106"/>
+      <c r="I157" s="106"/>
+      <c r="J157" s="106"/>
+      <c r="K157" s="106"/>
     </row>
     <row r="158" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A158" s="104" t="s">
+      <c r="A158" s="107" t="s">
         <v>126</v>
       </c>
-      <c r="B158" s="105"/>
-      <c r="C158" s="105"/>
-      <c r="D158" s="105"/>
-      <c r="E158" s="105"/>
-      <c r="F158" s="105"/>
-      <c r="G158" s="105"/>
-      <c r="H158" s="105"/>
-      <c r="I158" s="105"/>
-      <c r="J158" s="105"/>
-      <c r="K158" s="106"/>
+      <c r="B158" s="108"/>
+      <c r="C158" s="108"/>
+      <c r="D158" s="108"/>
+      <c r="E158" s="108"/>
+      <c r="F158" s="108"/>
+      <c r="G158" s="108"/>
+      <c r="H158" s="108"/>
+      <c r="I158" s="108"/>
+      <c r="J158" s="108"/>
+      <c r="K158" s="109"/>
     </row>
     <row r="159" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A159" s="3" t="s">
@@ -6228,7 +6252,7 @@
         <v>0</v>
       </c>
       <c r="F172" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G172" s="13" t="s">
         <v>11</v>
@@ -6243,45 +6267,45 @@
       </c>
     </row>
     <row r="173" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A173" s="102"/>
-      <c r="B173" s="102"/>
-      <c r="C173" s="102"/>
-      <c r="D173" s="102"/>
-      <c r="E173" s="102"/>
-      <c r="F173" s="102"/>
-      <c r="G173" s="102"/>
-      <c r="H173" s="102"/>
-      <c r="I173" s="102"/>
-      <c r="J173" s="102"/>
-      <c r="K173" s="102"/>
+      <c r="A173" s="105"/>
+      <c r="B173" s="105"/>
+      <c r="C173" s="105"/>
+      <c r="D173" s="105"/>
+      <c r="E173" s="105"/>
+      <c r="F173" s="105"/>
+      <c r="G173" s="105"/>
+      <c r="H173" s="105"/>
+      <c r="I173" s="105"/>
+      <c r="J173" s="105"/>
+      <c r="K173" s="105"/>
     </row>
     <row r="174" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A174" s="103"/>
-      <c r="B174" s="103"/>
-      <c r="C174" s="103"/>
-      <c r="D174" s="103"/>
-      <c r="E174" s="103"/>
-      <c r="F174" s="103"/>
-      <c r="G174" s="103"/>
-      <c r="H174" s="103"/>
-      <c r="I174" s="103"/>
-      <c r="J174" s="103"/>
-      <c r="K174" s="103"/>
+      <c r="A174" s="106"/>
+      <c r="B174" s="106"/>
+      <c r="C174" s="106"/>
+      <c r="D174" s="106"/>
+      <c r="E174" s="106"/>
+      <c r="F174" s="106"/>
+      <c r="G174" s="106"/>
+      <c r="H174" s="106"/>
+      <c r="I174" s="106"/>
+      <c r="J174" s="106"/>
+      <c r="K174" s="106"/>
     </row>
     <row r="175" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A175" s="104" t="s">
+      <c r="A175" s="107" t="s">
         <v>134</v>
       </c>
-      <c r="B175" s="105"/>
-      <c r="C175" s="105"/>
-      <c r="D175" s="105"/>
-      <c r="E175" s="105"/>
-      <c r="F175" s="105"/>
-      <c r="G175" s="105"/>
-      <c r="H175" s="105"/>
-      <c r="I175" s="105"/>
-      <c r="J175" s="105"/>
-      <c r="K175" s="106"/>
+      <c r="B175" s="108"/>
+      <c r="C175" s="108"/>
+      <c r="D175" s="108"/>
+      <c r="E175" s="108"/>
+      <c r="F175" s="108"/>
+      <c r="G175" s="108"/>
+      <c r="H175" s="108"/>
+      <c r="I175" s="108"/>
+      <c r="J175" s="108"/>
+      <c r="K175" s="109"/>
     </row>
     <row r="176" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A176" s="3" t="s">
@@ -6480,7 +6504,7 @@
         <v>0</v>
       </c>
       <c r="F182" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G182" s="13" t="s">
         <v>11</v>
@@ -6495,45 +6519,45 @@
       </c>
     </row>
     <row r="183" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A183" s="102"/>
-      <c r="B183" s="102"/>
-      <c r="C183" s="102"/>
-      <c r="D183" s="102"/>
-      <c r="E183" s="102"/>
-      <c r="F183" s="102"/>
-      <c r="G183" s="102"/>
-      <c r="H183" s="102"/>
-      <c r="I183" s="102"/>
-      <c r="J183" s="102"/>
-      <c r="K183" s="102"/>
+      <c r="A183" s="105"/>
+      <c r="B183" s="105"/>
+      <c r="C183" s="105"/>
+      <c r="D183" s="105"/>
+      <c r="E183" s="105"/>
+      <c r="F183" s="105"/>
+      <c r="G183" s="105"/>
+      <c r="H183" s="105"/>
+      <c r="I183" s="105"/>
+      <c r="J183" s="105"/>
+      <c r="K183" s="105"/>
     </row>
     <row r="184" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A184" s="103"/>
-      <c r="B184" s="103"/>
-      <c r="C184" s="103"/>
-      <c r="D184" s="103"/>
-      <c r="E184" s="103"/>
-      <c r="F184" s="103"/>
-      <c r="G184" s="103"/>
-      <c r="H184" s="103"/>
-      <c r="I184" s="103"/>
-      <c r="J184" s="103"/>
-      <c r="K184" s="103"/>
+      <c r="A184" s="106"/>
+      <c r="B184" s="106"/>
+      <c r="C184" s="106"/>
+      <c r="D184" s="106"/>
+      <c r="E184" s="106"/>
+      <c r="F184" s="106"/>
+      <c r="G184" s="106"/>
+      <c r="H184" s="106"/>
+      <c r="I184" s="106"/>
+      <c r="J184" s="106"/>
+      <c r="K184" s="106"/>
     </row>
     <row r="185" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A185" s="104" t="s">
+      <c r="A185" s="107" t="s">
         <v>69</v>
       </c>
-      <c r="B185" s="105"/>
-      <c r="C185" s="105"/>
-      <c r="D185" s="105"/>
-      <c r="E185" s="105"/>
-      <c r="F185" s="105"/>
-      <c r="G185" s="105"/>
-      <c r="H185" s="105"/>
-      <c r="I185" s="105"/>
-      <c r="J185" s="105"/>
-      <c r="K185" s="106"/>
+      <c r="B185" s="108"/>
+      <c r="C185" s="108"/>
+      <c r="D185" s="108"/>
+      <c r="E185" s="108"/>
+      <c r="F185" s="108"/>
+      <c r="G185" s="108"/>
+      <c r="H185" s="108"/>
+      <c r="I185" s="108"/>
+      <c r="J185" s="108"/>
+      <c r="K185" s="109"/>
     </row>
     <row r="186" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A186" s="3" t="s">
@@ -6801,7 +6825,7 @@
         <v>0</v>
       </c>
       <c r="F195" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G195" s="13" t="s">
         <v>11</v>
@@ -6816,45 +6840,45 @@
       </c>
     </row>
     <row r="196" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A196" s="102"/>
-      <c r="B196" s="102"/>
-      <c r="C196" s="102"/>
-      <c r="D196" s="102"/>
-      <c r="E196" s="102"/>
-      <c r="F196" s="102"/>
-      <c r="G196" s="102"/>
-      <c r="H196" s="102"/>
-      <c r="I196" s="102"/>
-      <c r="J196" s="102"/>
-      <c r="K196" s="102"/>
+      <c r="A196" s="105"/>
+      <c r="B196" s="105"/>
+      <c r="C196" s="105"/>
+      <c r="D196" s="105"/>
+      <c r="E196" s="105"/>
+      <c r="F196" s="105"/>
+      <c r="G196" s="105"/>
+      <c r="H196" s="105"/>
+      <c r="I196" s="105"/>
+      <c r="J196" s="105"/>
+      <c r="K196" s="105"/>
     </row>
     <row r="197" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A197" s="103"/>
-      <c r="B197" s="103"/>
-      <c r="C197" s="103"/>
-      <c r="D197" s="103"/>
-      <c r="E197" s="103"/>
-      <c r="F197" s="103"/>
-      <c r="G197" s="103"/>
-      <c r="H197" s="103"/>
-      <c r="I197" s="103"/>
-      <c r="J197" s="103"/>
-      <c r="K197" s="103"/>
+      <c r="A197" s="106"/>
+      <c r="B197" s="106"/>
+      <c r="C197" s="106"/>
+      <c r="D197" s="106"/>
+      <c r="E197" s="106"/>
+      <c r="F197" s="106"/>
+      <c r="G197" s="106"/>
+      <c r="H197" s="106"/>
+      <c r="I197" s="106"/>
+      <c r="J197" s="106"/>
+      <c r="K197" s="106"/>
     </row>
     <row r="198" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A198" s="104" t="s">
+      <c r="A198" s="107" t="s">
         <v>75</v>
       </c>
-      <c r="B198" s="105"/>
-      <c r="C198" s="105"/>
-      <c r="D198" s="105"/>
-      <c r="E198" s="105"/>
-      <c r="F198" s="105"/>
-      <c r="G198" s="105"/>
-      <c r="H198" s="105"/>
-      <c r="I198" s="105"/>
-      <c r="J198" s="105"/>
-      <c r="K198" s="106"/>
+      <c r="B198" s="108"/>
+      <c r="C198" s="108"/>
+      <c r="D198" s="108"/>
+      <c r="E198" s="108"/>
+      <c r="F198" s="108"/>
+      <c r="G198" s="108"/>
+      <c r="H198" s="108"/>
+      <c r="I198" s="108"/>
+      <c r="J198" s="108"/>
+      <c r="K198" s="109"/>
     </row>
     <row r="199" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A199" s="3" t="s">
@@ -7107,7 +7131,7 @@
         <v>0</v>
       </c>
       <c r="F207" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G207" s="13" t="s">
         <v>11</v>
@@ -7122,45 +7146,45 @@
       </c>
     </row>
     <row r="208" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A208" s="102"/>
-      <c r="B208" s="102"/>
-      <c r="C208" s="102"/>
-      <c r="D208" s="102"/>
-      <c r="E208" s="102"/>
-      <c r="F208" s="102"/>
-      <c r="G208" s="102"/>
-      <c r="H208" s="102"/>
-      <c r="I208" s="102"/>
-      <c r="J208" s="102"/>
-      <c r="K208" s="102"/>
+      <c r="A208" s="105"/>
+      <c r="B208" s="105"/>
+      <c r="C208" s="105"/>
+      <c r="D208" s="105"/>
+      <c r="E208" s="105"/>
+      <c r="F208" s="105"/>
+      <c r="G208" s="105"/>
+      <c r="H208" s="105"/>
+      <c r="I208" s="105"/>
+      <c r="J208" s="105"/>
+      <c r="K208" s="105"/>
     </row>
     <row r="209" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A209" s="103"/>
-      <c r="B209" s="103"/>
-      <c r="C209" s="103"/>
-      <c r="D209" s="103"/>
-      <c r="E209" s="103"/>
-      <c r="F209" s="103"/>
-      <c r="G209" s="103"/>
-      <c r="H209" s="103"/>
-      <c r="I209" s="103"/>
-      <c r="J209" s="103"/>
-      <c r="K209" s="103"/>
+      <c r="A209" s="106"/>
+      <c r="B209" s="106"/>
+      <c r="C209" s="106"/>
+      <c r="D209" s="106"/>
+      <c r="E209" s="106"/>
+      <c r="F209" s="106"/>
+      <c r="G209" s="106"/>
+      <c r="H209" s="106"/>
+      <c r="I209" s="106"/>
+      <c r="J209" s="106"/>
+      <c r="K209" s="106"/>
     </row>
     <row r="210" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A210" s="104" t="s">
+      <c r="A210" s="107" t="s">
         <v>83</v>
       </c>
-      <c r="B210" s="105"/>
-      <c r="C210" s="105"/>
-      <c r="D210" s="105"/>
-      <c r="E210" s="105"/>
-      <c r="F210" s="105"/>
-      <c r="G210" s="105"/>
-      <c r="H210" s="105"/>
-      <c r="I210" s="105"/>
-      <c r="J210" s="105"/>
-      <c r="K210" s="106"/>
+      <c r="B210" s="108"/>
+      <c r="C210" s="108"/>
+      <c r="D210" s="108"/>
+      <c r="E210" s="108"/>
+      <c r="F210" s="108"/>
+      <c r="G210" s="108"/>
+      <c r="H210" s="108"/>
+      <c r="I210" s="108"/>
+      <c r="J210" s="108"/>
+      <c r="K210" s="109"/>
     </row>
     <row r="211" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A211" s="3" t="s">
@@ -7415,7 +7439,7 @@
         <v>0</v>
       </c>
       <c r="F219" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G219" s="13" t="s">
         <v>11</v>
@@ -7430,45 +7454,45 @@
       </c>
     </row>
     <row r="220" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A220" s="102"/>
-      <c r="B220" s="102"/>
-      <c r="C220" s="102"/>
-      <c r="D220" s="102"/>
-      <c r="E220" s="102"/>
-      <c r="F220" s="102"/>
-      <c r="G220" s="102"/>
-      <c r="H220" s="102"/>
-      <c r="I220" s="102"/>
-      <c r="J220" s="102"/>
-      <c r="K220" s="102"/>
+      <c r="A220" s="105"/>
+      <c r="B220" s="105"/>
+      <c r="C220" s="105"/>
+      <c r="D220" s="105"/>
+      <c r="E220" s="105"/>
+      <c r="F220" s="105"/>
+      <c r="G220" s="105"/>
+      <c r="H220" s="105"/>
+      <c r="I220" s="105"/>
+      <c r="J220" s="105"/>
+      <c r="K220" s="105"/>
     </row>
     <row r="221" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A221" s="103"/>
-      <c r="B221" s="103"/>
-      <c r="C221" s="103"/>
-      <c r="D221" s="103"/>
-      <c r="E221" s="103"/>
-      <c r="F221" s="103"/>
-      <c r="G221" s="103"/>
-      <c r="H221" s="103"/>
-      <c r="I221" s="103"/>
-      <c r="J221" s="103"/>
-      <c r="K221" s="103"/>
+      <c r="A221" s="106"/>
+      <c r="B221" s="106"/>
+      <c r="C221" s="106"/>
+      <c r="D221" s="106"/>
+      <c r="E221" s="106"/>
+      <c r="F221" s="106"/>
+      <c r="G221" s="106"/>
+      <c r="H221" s="106"/>
+      <c r="I221" s="106"/>
+      <c r="J221" s="106"/>
+      <c r="K221" s="106"/>
     </row>
     <row r="222" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A222" s="104" t="s">
+      <c r="A222" s="107" t="s">
         <v>177</v>
       </c>
-      <c r="B222" s="105"/>
-      <c r="C222" s="105"/>
-      <c r="D222" s="105"/>
-      <c r="E222" s="105"/>
-      <c r="F222" s="105"/>
-      <c r="G222" s="105"/>
-      <c r="H222" s="105"/>
-      <c r="I222" s="105"/>
-      <c r="J222" s="105"/>
-      <c r="K222" s="106"/>
+      <c r="B222" s="108"/>
+      <c r="C222" s="108"/>
+      <c r="D222" s="108"/>
+      <c r="E222" s="108"/>
+      <c r="F222" s="108"/>
+      <c r="G222" s="108"/>
+      <c r="H222" s="108"/>
+      <c r="I222" s="108"/>
+      <c r="J222" s="108"/>
+      <c r="K222" s="109"/>
     </row>
     <row r="223" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A223" s="3" t="s">
@@ -7866,45 +7890,45 @@
       </c>
     </row>
     <row r="236" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A236" s="102"/>
-      <c r="B236" s="102"/>
-      <c r="C236" s="102"/>
-      <c r="D236" s="102"/>
-      <c r="E236" s="102"/>
-      <c r="F236" s="102"/>
-      <c r="G236" s="102"/>
-      <c r="H236" s="102"/>
-      <c r="I236" s="102"/>
-      <c r="J236" s="102"/>
-      <c r="K236" s="102"/>
+      <c r="A236" s="105"/>
+      <c r="B236" s="105"/>
+      <c r="C236" s="105"/>
+      <c r="D236" s="105"/>
+      <c r="E236" s="105"/>
+      <c r="F236" s="105"/>
+      <c r="G236" s="105"/>
+      <c r="H236" s="105"/>
+      <c r="I236" s="105"/>
+      <c r="J236" s="105"/>
+      <c r="K236" s="105"/>
     </row>
     <row r="237" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A237" s="103"/>
-      <c r="B237" s="103"/>
-      <c r="C237" s="103"/>
-      <c r="D237" s="103"/>
-      <c r="E237" s="103"/>
-      <c r="F237" s="103"/>
-      <c r="G237" s="103"/>
-      <c r="H237" s="103"/>
-      <c r="I237" s="103"/>
-      <c r="J237" s="103"/>
-      <c r="K237" s="103"/>
+      <c r="A237" s="106"/>
+      <c r="B237" s="106"/>
+      <c r="C237" s="106"/>
+      <c r="D237" s="106"/>
+      <c r="E237" s="106"/>
+      <c r="F237" s="106"/>
+      <c r="G237" s="106"/>
+      <c r="H237" s="106"/>
+      <c r="I237" s="106"/>
+      <c r="J237" s="106"/>
+      <c r="K237" s="106"/>
     </row>
     <row r="238" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A238" s="104" t="s">
+      <c r="A238" s="107" t="s">
         <v>200</v>
       </c>
-      <c r="B238" s="105"/>
-      <c r="C238" s="105"/>
-      <c r="D238" s="105"/>
-      <c r="E238" s="105"/>
-      <c r="F238" s="105"/>
-      <c r="G238" s="105"/>
-      <c r="H238" s="105"/>
-      <c r="I238" s="105"/>
-      <c r="J238" s="105"/>
-      <c r="K238" s="106"/>
+      <c r="B238" s="108"/>
+      <c r="C238" s="108"/>
+      <c r="D238" s="108"/>
+      <c r="E238" s="108"/>
+      <c r="F238" s="108"/>
+      <c r="G238" s="108"/>
+      <c r="H238" s="108"/>
+      <c r="I238" s="108"/>
+      <c r="J238" s="108"/>
+      <c r="K238" s="109"/>
     </row>
     <row r="239" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A239" s="3" t="s">
@@ -8090,7 +8114,7 @@
         <v>0</v>
       </c>
       <c r="F245" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G245" s="13" t="s">
         <v>11</v>
@@ -8105,45 +8129,45 @@
       </c>
     </row>
     <row r="246" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A246" s="102"/>
-      <c r="B246" s="102"/>
-      <c r="C246" s="102"/>
-      <c r="D246" s="102"/>
-      <c r="E246" s="102"/>
-      <c r="F246" s="102"/>
-      <c r="G246" s="102"/>
-      <c r="H246" s="102"/>
-      <c r="I246" s="102"/>
-      <c r="J246" s="102"/>
-      <c r="K246" s="102"/>
+      <c r="A246" s="105"/>
+      <c r="B246" s="105"/>
+      <c r="C246" s="105"/>
+      <c r="D246" s="105"/>
+      <c r="E246" s="105"/>
+      <c r="F246" s="105"/>
+      <c r="G246" s="105"/>
+      <c r="H246" s="105"/>
+      <c r="I246" s="105"/>
+      <c r="J246" s="105"/>
+      <c r="K246" s="105"/>
     </row>
     <row r="247" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A247" s="103"/>
-      <c r="B247" s="103"/>
-      <c r="C247" s="103"/>
-      <c r="D247" s="103"/>
-      <c r="E247" s="103"/>
-      <c r="F247" s="103"/>
-      <c r="G247" s="103"/>
-      <c r="H247" s="103"/>
-      <c r="I247" s="103"/>
-      <c r="J247" s="103"/>
-      <c r="K247" s="103"/>
+      <c r="A247" s="106"/>
+      <c r="B247" s="106"/>
+      <c r="C247" s="106"/>
+      <c r="D247" s="106"/>
+      <c r="E247" s="106"/>
+      <c r="F247" s="106"/>
+      <c r="G247" s="106"/>
+      <c r="H247" s="106"/>
+      <c r="I247" s="106"/>
+      <c r="J247" s="106"/>
+      <c r="K247" s="106"/>
     </row>
     <row r="248" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A248" s="104" t="s">
+      <c r="A248" s="107" t="s">
         <v>203</v>
       </c>
-      <c r="B248" s="105"/>
-      <c r="C248" s="105"/>
-      <c r="D248" s="105"/>
-      <c r="E248" s="105"/>
-      <c r="F248" s="105"/>
-      <c r="G248" s="105"/>
-      <c r="H248" s="105"/>
-      <c r="I248" s="105"/>
-      <c r="J248" s="105"/>
-      <c r="K248" s="106"/>
+      <c r="B248" s="108"/>
+      <c r="C248" s="108"/>
+      <c r="D248" s="108"/>
+      <c r="E248" s="108"/>
+      <c r="F248" s="108"/>
+      <c r="G248" s="108"/>
+      <c r="H248" s="108"/>
+      <c r="I248" s="108"/>
+      <c r="J248" s="108"/>
+      <c r="K248" s="109"/>
     </row>
     <row r="249" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A249" s="3" t="s">
@@ -8375,7 +8399,7 @@
         <v>0</v>
       </c>
       <c r="F256" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G256" s="13" t="s">
         <v>11</v>
@@ -8390,45 +8414,45 @@
       </c>
     </row>
     <row r="257" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A257" s="102"/>
-      <c r="B257" s="102"/>
-      <c r="C257" s="102"/>
-      <c r="D257" s="102"/>
-      <c r="E257" s="102"/>
-      <c r="F257" s="102"/>
-      <c r="G257" s="102"/>
-      <c r="H257" s="102"/>
-      <c r="I257" s="102"/>
-      <c r="J257" s="102"/>
-      <c r="K257" s="102"/>
+      <c r="A257" s="105"/>
+      <c r="B257" s="105"/>
+      <c r="C257" s="105"/>
+      <c r="D257" s="105"/>
+      <c r="E257" s="105"/>
+      <c r="F257" s="105"/>
+      <c r="G257" s="105"/>
+      <c r="H257" s="105"/>
+      <c r="I257" s="105"/>
+      <c r="J257" s="105"/>
+      <c r="K257" s="105"/>
     </row>
     <row r="258" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A258" s="103"/>
-      <c r="B258" s="103"/>
-      <c r="C258" s="103"/>
-      <c r="D258" s="103"/>
-      <c r="E258" s="103"/>
-      <c r="F258" s="103"/>
-      <c r="G258" s="103"/>
-      <c r="H258" s="103"/>
-      <c r="I258" s="103"/>
-      <c r="J258" s="103"/>
-      <c r="K258" s="103"/>
+      <c r="A258" s="106"/>
+      <c r="B258" s="106"/>
+      <c r="C258" s="106"/>
+      <c r="D258" s="106"/>
+      <c r="E258" s="106"/>
+      <c r="F258" s="106"/>
+      <c r="G258" s="106"/>
+      <c r="H258" s="106"/>
+      <c r="I258" s="106"/>
+      <c r="J258" s="106"/>
+      <c r="K258" s="106"/>
     </row>
     <row r="259" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A259" s="104" t="s">
+      <c r="A259" s="107" t="s">
         <v>207</v>
       </c>
-      <c r="B259" s="105"/>
-      <c r="C259" s="105"/>
-      <c r="D259" s="105"/>
-      <c r="E259" s="105"/>
-      <c r="F259" s="105"/>
-      <c r="G259" s="105"/>
-      <c r="H259" s="105"/>
-      <c r="I259" s="105"/>
-      <c r="J259" s="105"/>
-      <c r="K259" s="106"/>
+      <c r="B259" s="108"/>
+      <c r="C259" s="108"/>
+      <c r="D259" s="108"/>
+      <c r="E259" s="108"/>
+      <c r="F259" s="108"/>
+      <c r="G259" s="108"/>
+      <c r="H259" s="108"/>
+      <c r="I259" s="108"/>
+      <c r="J259" s="108"/>
+      <c r="K259" s="109"/>
     </row>
     <row r="260" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A260" s="3" t="s">
@@ -8656,7 +8680,7 @@
         <v>0</v>
       </c>
       <c r="F267" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G267" s="13" t="s">
         <v>11</v>
@@ -8671,45 +8695,45 @@
       </c>
     </row>
     <row r="268" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A268" s="102"/>
-      <c r="B268" s="102"/>
-      <c r="C268" s="102"/>
-      <c r="D268" s="102"/>
-      <c r="E268" s="102"/>
-      <c r="F268" s="102"/>
-      <c r="G268" s="102"/>
-      <c r="H268" s="102"/>
-      <c r="I268" s="102"/>
-      <c r="J268" s="102"/>
-      <c r="K268" s="102"/>
+      <c r="A268" s="105"/>
+      <c r="B268" s="105"/>
+      <c r="C268" s="105"/>
+      <c r="D268" s="105"/>
+      <c r="E268" s="105"/>
+      <c r="F268" s="105"/>
+      <c r="G268" s="105"/>
+      <c r="H268" s="105"/>
+      <c r="I268" s="105"/>
+      <c r="J268" s="105"/>
+      <c r="K268" s="105"/>
     </row>
     <row r="269" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A269" s="103"/>
-      <c r="B269" s="103"/>
-      <c r="C269" s="103"/>
-      <c r="D269" s="103"/>
-      <c r="E269" s="103"/>
-      <c r="F269" s="103"/>
-      <c r="G269" s="103"/>
-      <c r="H269" s="103"/>
-      <c r="I269" s="103"/>
-      <c r="J269" s="103"/>
-      <c r="K269" s="103"/>
+      <c r="A269" s="106"/>
+      <c r="B269" s="106"/>
+      <c r="C269" s="106"/>
+      <c r="D269" s="106"/>
+      <c r="E269" s="106"/>
+      <c r="F269" s="106"/>
+      <c r="G269" s="106"/>
+      <c r="H269" s="106"/>
+      <c r="I269" s="106"/>
+      <c r="J269" s="106"/>
+      <c r="K269" s="106"/>
     </row>
     <row r="270" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A270" s="104" t="s">
+      <c r="A270" s="107" t="s">
         <v>238</v>
       </c>
-      <c r="B270" s="105"/>
-      <c r="C270" s="105"/>
-      <c r="D270" s="105"/>
-      <c r="E270" s="105"/>
-      <c r="F270" s="105"/>
-      <c r="G270" s="105"/>
-      <c r="H270" s="105"/>
-      <c r="I270" s="105"/>
-      <c r="J270" s="105"/>
-      <c r="K270" s="106"/>
+      <c r="B270" s="108"/>
+      <c r="C270" s="108"/>
+      <c r="D270" s="108"/>
+      <c r="E270" s="108"/>
+      <c r="F270" s="108"/>
+      <c r="G270" s="108"/>
+      <c r="H270" s="108"/>
+      <c r="I270" s="108"/>
+      <c r="J270" s="108"/>
+      <c r="K270" s="109"/>
     </row>
     <row r="271" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A271" s="3" t="s">
@@ -8877,7 +8901,7 @@
         <v>0</v>
       </c>
       <c r="F276" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G276" s="13" t="s">
         <v>11</v>
@@ -8892,45 +8916,45 @@
       </c>
     </row>
     <row r="277" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A277" s="102"/>
-      <c r="B277" s="102"/>
-      <c r="C277" s="102"/>
-      <c r="D277" s="102"/>
-      <c r="E277" s="102"/>
-      <c r="F277" s="102"/>
-      <c r="G277" s="102"/>
-      <c r="H277" s="102"/>
-      <c r="I277" s="102"/>
-      <c r="J277" s="102"/>
-      <c r="K277" s="102"/>
+      <c r="A277" s="105"/>
+      <c r="B277" s="105"/>
+      <c r="C277" s="105"/>
+      <c r="D277" s="105"/>
+      <c r="E277" s="105"/>
+      <c r="F277" s="105"/>
+      <c r="G277" s="105"/>
+      <c r="H277" s="105"/>
+      <c r="I277" s="105"/>
+      <c r="J277" s="105"/>
+      <c r="K277" s="105"/>
     </row>
     <row r="278" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A278" s="103"/>
-      <c r="B278" s="103"/>
-      <c r="C278" s="103"/>
-      <c r="D278" s="103"/>
-      <c r="E278" s="103"/>
-      <c r="F278" s="103"/>
-      <c r="G278" s="103"/>
-      <c r="H278" s="103"/>
-      <c r="I278" s="103"/>
-      <c r="J278" s="103"/>
-      <c r="K278" s="103"/>
+      <c r="A278" s="106"/>
+      <c r="B278" s="106"/>
+      <c r="C278" s="106"/>
+      <c r="D278" s="106"/>
+      <c r="E278" s="106"/>
+      <c r="F278" s="106"/>
+      <c r="G278" s="106"/>
+      <c r="H278" s="106"/>
+      <c r="I278" s="106"/>
+      <c r="J278" s="106"/>
+      <c r="K278" s="106"/>
     </row>
     <row r="279" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A279" s="104" t="s">
+      <c r="A279" s="107" t="s">
         <v>240</v>
       </c>
-      <c r="B279" s="105"/>
-      <c r="C279" s="105"/>
-      <c r="D279" s="105"/>
-      <c r="E279" s="105"/>
-      <c r="F279" s="105"/>
-      <c r="G279" s="105"/>
-      <c r="H279" s="105"/>
-      <c r="I279" s="105"/>
-      <c r="J279" s="105"/>
-      <c r="K279" s="106"/>
+      <c r="B279" s="108"/>
+      <c r="C279" s="108"/>
+      <c r="D279" s="108"/>
+      <c r="E279" s="108"/>
+      <c r="F279" s="108"/>
+      <c r="G279" s="108"/>
+      <c r="H279" s="108"/>
+      <c r="I279" s="108"/>
+      <c r="J279" s="108"/>
+      <c r="K279" s="109"/>
     </row>
     <row r="280" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A280" s="3" t="s">
@@ -9098,7 +9122,7 @@
         <v>0</v>
       </c>
       <c r="F285" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G285" s="13" t="s">
         <v>11</v>
@@ -9113,45 +9137,45 @@
       </c>
     </row>
     <row r="286" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A286" s="102"/>
-      <c r="B286" s="102"/>
-      <c r="C286" s="102"/>
-      <c r="D286" s="102"/>
-      <c r="E286" s="102"/>
-      <c r="F286" s="102"/>
-      <c r="G286" s="102"/>
-      <c r="H286" s="102"/>
-      <c r="I286" s="102"/>
-      <c r="J286" s="102"/>
-      <c r="K286" s="102"/>
+      <c r="A286" s="105"/>
+      <c r="B286" s="105"/>
+      <c r="C286" s="105"/>
+      <c r="D286" s="105"/>
+      <c r="E286" s="105"/>
+      <c r="F286" s="105"/>
+      <c r="G286" s="105"/>
+      <c r="H286" s="105"/>
+      <c r="I286" s="105"/>
+      <c r="J286" s="105"/>
+      <c r="K286" s="105"/>
     </row>
     <row r="287" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A287" s="103"/>
-      <c r="B287" s="103"/>
-      <c r="C287" s="103"/>
-      <c r="D287" s="103"/>
-      <c r="E287" s="103"/>
-      <c r="F287" s="103"/>
-      <c r="G287" s="103"/>
-      <c r="H287" s="103"/>
-      <c r="I287" s="103"/>
-      <c r="J287" s="103"/>
-      <c r="K287" s="103"/>
+      <c r="A287" s="106"/>
+      <c r="B287" s="106"/>
+      <c r="C287" s="106"/>
+      <c r="D287" s="106"/>
+      <c r="E287" s="106"/>
+      <c r="F287" s="106"/>
+      <c r="G287" s="106"/>
+      <c r="H287" s="106"/>
+      <c r="I287" s="106"/>
+      <c r="J287" s="106"/>
+      <c r="K287" s="106"/>
     </row>
     <row r="288" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A288" s="104" t="s">
+      <c r="A288" s="107" t="s">
         <v>242</v>
       </c>
-      <c r="B288" s="105"/>
-      <c r="C288" s="105"/>
-      <c r="D288" s="105"/>
-      <c r="E288" s="105"/>
-      <c r="F288" s="105"/>
-      <c r="G288" s="105"/>
-      <c r="H288" s="105"/>
-      <c r="I288" s="105"/>
-      <c r="J288" s="105"/>
-      <c r="K288" s="106"/>
+      <c r="B288" s="108"/>
+      <c r="C288" s="108"/>
+      <c r="D288" s="108"/>
+      <c r="E288" s="108"/>
+      <c r="F288" s="108"/>
+      <c r="G288" s="108"/>
+      <c r="H288" s="108"/>
+      <c r="I288" s="108"/>
+      <c r="J288" s="108"/>
+      <c r="K288" s="109"/>
     </row>
     <row r="289" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A289" s="3" t="s">
@@ -9319,7 +9343,7 @@
         <v>0</v>
       </c>
       <c r="F294" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G294" s="13" t="s">
         <v>11</v>
@@ -9334,45 +9358,45 @@
       </c>
     </row>
     <row r="295" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A295" s="102"/>
-      <c r="B295" s="102"/>
-      <c r="C295" s="102"/>
-      <c r="D295" s="102"/>
-      <c r="E295" s="102"/>
-      <c r="F295" s="102"/>
-      <c r="G295" s="102"/>
-      <c r="H295" s="102"/>
-      <c r="I295" s="102"/>
-      <c r="J295" s="102"/>
-      <c r="K295" s="102"/>
+      <c r="A295" s="105"/>
+      <c r="B295" s="105"/>
+      <c r="C295" s="105"/>
+      <c r="D295" s="105"/>
+      <c r="E295" s="105"/>
+      <c r="F295" s="105"/>
+      <c r="G295" s="105"/>
+      <c r="H295" s="105"/>
+      <c r="I295" s="105"/>
+      <c r="J295" s="105"/>
+      <c r="K295" s="105"/>
     </row>
     <row r="296" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A296" s="103"/>
-      <c r="B296" s="103"/>
-      <c r="C296" s="103"/>
-      <c r="D296" s="103"/>
-      <c r="E296" s="103"/>
-      <c r="F296" s="103"/>
-      <c r="G296" s="103"/>
-      <c r="H296" s="103"/>
-      <c r="I296" s="103"/>
-      <c r="J296" s="103"/>
-      <c r="K296" s="103"/>
+      <c r="A296" s="106"/>
+      <c r="B296" s="106"/>
+      <c r="C296" s="106"/>
+      <c r="D296" s="106"/>
+      <c r="E296" s="106"/>
+      <c r="F296" s="106"/>
+      <c r="G296" s="106"/>
+      <c r="H296" s="106"/>
+      <c r="I296" s="106"/>
+      <c r="J296" s="106"/>
+      <c r="K296" s="106"/>
     </row>
     <row r="297" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A297" s="104" t="s">
+      <c r="A297" s="107" t="s">
         <v>244</v>
       </c>
-      <c r="B297" s="105"/>
-      <c r="C297" s="105"/>
-      <c r="D297" s="105"/>
-      <c r="E297" s="105"/>
-      <c r="F297" s="105"/>
-      <c r="G297" s="105"/>
-      <c r="H297" s="105"/>
-      <c r="I297" s="105"/>
-      <c r="J297" s="105"/>
-      <c r="K297" s="106"/>
+      <c r="B297" s="108"/>
+      <c r="C297" s="108"/>
+      <c r="D297" s="108"/>
+      <c r="E297" s="108"/>
+      <c r="F297" s="108"/>
+      <c r="G297" s="108"/>
+      <c r="H297" s="108"/>
+      <c r="I297" s="108"/>
+      <c r="J297" s="108"/>
+      <c r="K297" s="109"/>
     </row>
     <row r="298" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A298" s="3" t="s">
@@ -9540,7 +9564,7 @@
         <v>0</v>
       </c>
       <c r="F303" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G303" s="13" t="s">
         <v>11</v>
@@ -9555,45 +9579,45 @@
       </c>
     </row>
     <row r="304" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A304" s="102"/>
-      <c r="B304" s="102"/>
-      <c r="C304" s="102"/>
-      <c r="D304" s="102"/>
-      <c r="E304" s="102"/>
-      <c r="F304" s="102"/>
-      <c r="G304" s="102"/>
-      <c r="H304" s="102"/>
-      <c r="I304" s="102"/>
-      <c r="J304" s="102"/>
-      <c r="K304" s="102"/>
+      <c r="A304" s="105"/>
+      <c r="B304" s="105"/>
+      <c r="C304" s="105"/>
+      <c r="D304" s="105"/>
+      <c r="E304" s="105"/>
+      <c r="F304" s="105"/>
+      <c r="G304" s="105"/>
+      <c r="H304" s="105"/>
+      <c r="I304" s="105"/>
+      <c r="J304" s="105"/>
+      <c r="K304" s="105"/>
     </row>
     <row r="305" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A305" s="103"/>
-      <c r="B305" s="103"/>
-      <c r="C305" s="103"/>
-      <c r="D305" s="103"/>
-      <c r="E305" s="103"/>
-      <c r="F305" s="103"/>
-      <c r="G305" s="103"/>
-      <c r="H305" s="103"/>
-      <c r="I305" s="103"/>
-      <c r="J305" s="103"/>
-      <c r="K305" s="103"/>
+      <c r="A305" s="106"/>
+      <c r="B305" s="106"/>
+      <c r="C305" s="106"/>
+      <c r="D305" s="106"/>
+      <c r="E305" s="106"/>
+      <c r="F305" s="106"/>
+      <c r="G305" s="106"/>
+      <c r="H305" s="106"/>
+      <c r="I305" s="106"/>
+      <c r="J305" s="106"/>
+      <c r="K305" s="106"/>
     </row>
     <row r="306" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A306" s="104" t="s">
+      <c r="A306" s="107" t="s">
         <v>211</v>
       </c>
-      <c r="B306" s="105"/>
-      <c r="C306" s="105"/>
-      <c r="D306" s="105"/>
-      <c r="E306" s="105"/>
-      <c r="F306" s="105"/>
-      <c r="G306" s="105"/>
-      <c r="H306" s="105"/>
-      <c r="I306" s="105"/>
-      <c r="J306" s="105"/>
-      <c r="K306" s="106"/>
+      <c r="B306" s="108"/>
+      <c r="C306" s="108"/>
+      <c r="D306" s="108"/>
+      <c r="E306" s="108"/>
+      <c r="F306" s="108"/>
+      <c r="G306" s="108"/>
+      <c r="H306" s="108"/>
+      <c r="I306" s="108"/>
+      <c r="J306" s="108"/>
+      <c r="K306" s="109"/>
     </row>
     <row r="307" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A307" s="3" t="s">
@@ -9877,7 +9901,7 @@
         <v>0</v>
       </c>
       <c r="F317" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G317" s="13" t="s">
         <v>11</v>
@@ -9892,45 +9916,45 @@
       </c>
     </row>
     <row r="318" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A318" s="102"/>
-      <c r="B318" s="102"/>
-      <c r="C318" s="102"/>
-      <c r="D318" s="102"/>
-      <c r="E318" s="102"/>
-      <c r="F318" s="102"/>
-      <c r="G318" s="102"/>
-      <c r="H318" s="102"/>
-      <c r="I318" s="102"/>
-      <c r="J318" s="102"/>
-      <c r="K318" s="102"/>
+      <c r="A318" s="105"/>
+      <c r="B318" s="105"/>
+      <c r="C318" s="105"/>
+      <c r="D318" s="105"/>
+      <c r="E318" s="105"/>
+      <c r="F318" s="105"/>
+      <c r="G318" s="105"/>
+      <c r="H318" s="105"/>
+      <c r="I318" s="105"/>
+      <c r="J318" s="105"/>
+      <c r="K318" s="105"/>
     </row>
     <row r="319" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A319" s="103"/>
-      <c r="B319" s="103"/>
-      <c r="C319" s="103"/>
-      <c r="D319" s="103"/>
-      <c r="E319" s="103"/>
-      <c r="F319" s="103"/>
-      <c r="G319" s="103"/>
-      <c r="H319" s="103"/>
-      <c r="I319" s="103"/>
-      <c r="J319" s="103"/>
-      <c r="K319" s="103"/>
+      <c r="A319" s="106"/>
+      <c r="B319" s="106"/>
+      <c r="C319" s="106"/>
+      <c r="D319" s="106"/>
+      <c r="E319" s="106"/>
+      <c r="F319" s="106"/>
+      <c r="G319" s="106"/>
+      <c r="H319" s="106"/>
+      <c r="I319" s="106"/>
+      <c r="J319" s="106"/>
+      <c r="K319" s="106"/>
     </row>
     <row r="320" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A320" s="104" t="s">
+      <c r="A320" s="107" t="s">
         <v>214</v>
       </c>
-      <c r="B320" s="105"/>
-      <c r="C320" s="105"/>
-      <c r="D320" s="105"/>
-      <c r="E320" s="105"/>
-      <c r="F320" s="105"/>
-      <c r="G320" s="105"/>
-      <c r="H320" s="105"/>
-      <c r="I320" s="105"/>
-      <c r="J320" s="105"/>
-      <c r="K320" s="106"/>
+      <c r="B320" s="108"/>
+      <c r="C320" s="108"/>
+      <c r="D320" s="108"/>
+      <c r="E320" s="108"/>
+      <c r="F320" s="108"/>
+      <c r="G320" s="108"/>
+      <c r="H320" s="108"/>
+      <c r="I320" s="108"/>
+      <c r="J320" s="108"/>
+      <c r="K320" s="109"/>
     </row>
     <row r="321" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A321" s="3" t="s">
@@ -10162,7 +10186,7 @@
         <v>0</v>
       </c>
       <c r="F328" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G328" s="13" t="s">
         <v>11</v>
@@ -10177,45 +10201,45 @@
       </c>
     </row>
     <row r="329" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A329" s="102"/>
-      <c r="B329" s="102"/>
-      <c r="C329" s="102"/>
-      <c r="D329" s="102"/>
-      <c r="E329" s="102"/>
-      <c r="F329" s="102"/>
-      <c r="G329" s="102"/>
-      <c r="H329" s="102"/>
-      <c r="I329" s="102"/>
-      <c r="J329" s="102"/>
-      <c r="K329" s="102"/>
+      <c r="A329" s="105"/>
+      <c r="B329" s="105"/>
+      <c r="C329" s="105"/>
+      <c r="D329" s="105"/>
+      <c r="E329" s="105"/>
+      <c r="F329" s="105"/>
+      <c r="G329" s="105"/>
+      <c r="H329" s="105"/>
+      <c r="I329" s="105"/>
+      <c r="J329" s="105"/>
+      <c r="K329" s="105"/>
     </row>
     <row r="330" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A330" s="103"/>
-      <c r="B330" s="103"/>
-      <c r="C330" s="103"/>
-      <c r="D330" s="103"/>
-      <c r="E330" s="103"/>
-      <c r="F330" s="103"/>
-      <c r="G330" s="103"/>
-      <c r="H330" s="103"/>
-      <c r="I330" s="103"/>
-      <c r="J330" s="103"/>
-      <c r="K330" s="103"/>
+      <c r="A330" s="106"/>
+      <c r="B330" s="106"/>
+      <c r="C330" s="106"/>
+      <c r="D330" s="106"/>
+      <c r="E330" s="106"/>
+      <c r="F330" s="106"/>
+      <c r="G330" s="106"/>
+      <c r="H330" s="106"/>
+      <c r="I330" s="106"/>
+      <c r="J330" s="106"/>
+      <c r="K330" s="106"/>
     </row>
     <row r="331" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A331" s="104" t="s">
+      <c r="A331" s="107" t="s">
         <v>223</v>
       </c>
-      <c r="B331" s="105"/>
-      <c r="C331" s="105"/>
-      <c r="D331" s="105"/>
-      <c r="E331" s="105"/>
-      <c r="F331" s="105"/>
-      <c r="G331" s="105"/>
-      <c r="H331" s="105"/>
-      <c r="I331" s="105"/>
-      <c r="J331" s="105"/>
-      <c r="K331" s="106"/>
+      <c r="B331" s="108"/>
+      <c r="C331" s="108"/>
+      <c r="D331" s="108"/>
+      <c r="E331" s="108"/>
+      <c r="F331" s="108"/>
+      <c r="G331" s="108"/>
+      <c r="H331" s="108"/>
+      <c r="I331" s="108"/>
+      <c r="J331" s="108"/>
+      <c r="K331" s="109"/>
     </row>
     <row r="332" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A332" s="3" t="s">
@@ -10443,7 +10467,7 @@
         <v>0</v>
       </c>
       <c r="F339" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G339" s="13" t="s">
         <v>11</v>
@@ -10458,45 +10482,45 @@
       </c>
     </row>
     <row r="340" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A340" s="102"/>
-      <c r="B340" s="102"/>
-      <c r="C340" s="102"/>
-      <c r="D340" s="102"/>
-      <c r="E340" s="102"/>
-      <c r="F340" s="102"/>
-      <c r="G340" s="102"/>
-      <c r="H340" s="102"/>
-      <c r="I340" s="102"/>
-      <c r="J340" s="102"/>
-      <c r="K340" s="102"/>
+      <c r="A340" s="105"/>
+      <c r="B340" s="105"/>
+      <c r="C340" s="105"/>
+      <c r="D340" s="105"/>
+      <c r="E340" s="105"/>
+      <c r="F340" s="105"/>
+      <c r="G340" s="105"/>
+      <c r="H340" s="105"/>
+      <c r="I340" s="105"/>
+      <c r="J340" s="105"/>
+      <c r="K340" s="105"/>
     </row>
     <row r="341" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A341" s="103"/>
-      <c r="B341" s="103"/>
-      <c r="C341" s="103"/>
-      <c r="D341" s="103"/>
-      <c r="E341" s="103"/>
-      <c r="F341" s="103"/>
-      <c r="G341" s="103"/>
-      <c r="H341" s="103"/>
-      <c r="I341" s="103"/>
-      <c r="J341" s="103"/>
-      <c r="K341" s="103"/>
+      <c r="A341" s="106"/>
+      <c r="B341" s="106"/>
+      <c r="C341" s="106"/>
+      <c r="D341" s="106"/>
+      <c r="E341" s="106"/>
+      <c r="F341" s="106"/>
+      <c r="G341" s="106"/>
+      <c r="H341" s="106"/>
+      <c r="I341" s="106"/>
+      <c r="J341" s="106"/>
+      <c r="K341" s="106"/>
     </row>
     <row r="342" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A342" s="104" t="s">
+      <c r="A342" s="107" t="s">
         <v>234</v>
       </c>
-      <c r="B342" s="105"/>
-      <c r="C342" s="105"/>
-      <c r="D342" s="105"/>
-      <c r="E342" s="105"/>
-      <c r="F342" s="105"/>
-      <c r="G342" s="105"/>
-      <c r="H342" s="105"/>
-      <c r="I342" s="105"/>
-      <c r="J342" s="105"/>
-      <c r="K342" s="106"/>
+      <c r="B342" s="108"/>
+      <c r="C342" s="108"/>
+      <c r="D342" s="108"/>
+      <c r="E342" s="108"/>
+      <c r="F342" s="108"/>
+      <c r="G342" s="108"/>
+      <c r="H342" s="108"/>
+      <c r="I342" s="108"/>
+      <c r="J342" s="108"/>
+      <c r="K342" s="109"/>
     </row>
     <row r="343" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A343" s="3" t="s">
@@ -10716,7 +10740,7 @@
         <v>0</v>
       </c>
       <c r="F350" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G350" s="13" t="s">
         <v>11</v>
@@ -10731,45 +10755,45 @@
       </c>
     </row>
     <row r="351" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A351" s="102"/>
-      <c r="B351" s="102"/>
-      <c r="C351" s="102"/>
-      <c r="D351" s="102"/>
-      <c r="E351" s="102"/>
-      <c r="F351" s="102"/>
-      <c r="G351" s="102"/>
-      <c r="H351" s="102"/>
-      <c r="I351" s="102"/>
-      <c r="J351" s="102"/>
-      <c r="K351" s="102"/>
+      <c r="A351" s="105"/>
+      <c r="B351" s="105"/>
+      <c r="C351" s="105"/>
+      <c r="D351" s="105"/>
+      <c r="E351" s="105"/>
+      <c r="F351" s="105"/>
+      <c r="G351" s="105"/>
+      <c r="H351" s="105"/>
+      <c r="I351" s="105"/>
+      <c r="J351" s="105"/>
+      <c r="K351" s="105"/>
     </row>
     <row r="352" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A352" s="103"/>
-      <c r="B352" s="103"/>
-      <c r="C352" s="103"/>
-      <c r="D352" s="103"/>
-      <c r="E352" s="103"/>
-      <c r="F352" s="103"/>
-      <c r="G352" s="103"/>
-      <c r="H352" s="103"/>
-      <c r="I352" s="103"/>
-      <c r="J352" s="103"/>
-      <c r="K352" s="103"/>
+      <c r="A352" s="106"/>
+      <c r="B352" s="106"/>
+      <c r="C352" s="106"/>
+      <c r="D352" s="106"/>
+      <c r="E352" s="106"/>
+      <c r="F352" s="106"/>
+      <c r="G352" s="106"/>
+      <c r="H352" s="106"/>
+      <c r="I352" s="106"/>
+      <c r="J352" s="106"/>
+      <c r="K352" s="106"/>
     </row>
     <row r="353" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A353" s="104" t="s">
+      <c r="A353" s="107" t="s">
         <v>121</v>
       </c>
-      <c r="B353" s="105"/>
-      <c r="C353" s="105"/>
-      <c r="D353" s="105"/>
-      <c r="E353" s="105"/>
-      <c r="F353" s="105"/>
-      <c r="G353" s="105"/>
-      <c r="H353" s="105"/>
-      <c r="I353" s="105"/>
-      <c r="J353" s="105"/>
-      <c r="K353" s="106"/>
+      <c r="B353" s="108"/>
+      <c r="C353" s="108"/>
+      <c r="D353" s="108"/>
+      <c r="E353" s="108"/>
+      <c r="F353" s="108"/>
+      <c r="G353" s="108"/>
+      <c r="H353" s="108"/>
+      <c r="I353" s="108"/>
+      <c r="J353" s="108"/>
+      <c r="K353" s="109"/>
     </row>
     <row r="354" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A354" s="3" t="s">
@@ -11074,7 +11098,7 @@
         <v>0</v>
       </c>
       <c r="F364" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G364" s="13" t="s">
         <v>11</v>
@@ -11089,45 +11113,45 @@
       </c>
     </row>
     <row r="365" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A365" s="102"/>
-      <c r="B365" s="102"/>
-      <c r="C365" s="102"/>
-      <c r="D365" s="102"/>
-      <c r="E365" s="102"/>
-      <c r="F365" s="102"/>
-      <c r="G365" s="102"/>
-      <c r="H365" s="102"/>
-      <c r="I365" s="102"/>
-      <c r="J365" s="102"/>
-      <c r="K365" s="102"/>
+      <c r="A365" s="105"/>
+      <c r="B365" s="105"/>
+      <c r="C365" s="105"/>
+      <c r="D365" s="105"/>
+      <c r="E365" s="105"/>
+      <c r="F365" s="105"/>
+      <c r="G365" s="105"/>
+      <c r="H365" s="105"/>
+      <c r="I365" s="105"/>
+      <c r="J365" s="105"/>
+      <c r="K365" s="105"/>
     </row>
     <row r="366" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A366" s="103"/>
-      <c r="B366" s="103"/>
-      <c r="C366" s="103"/>
-      <c r="D366" s="103"/>
-      <c r="E366" s="103"/>
-      <c r="F366" s="103"/>
-      <c r="G366" s="103"/>
-      <c r="H366" s="103"/>
-      <c r="I366" s="103"/>
-      <c r="J366" s="103"/>
-      <c r="K366" s="103"/>
+      <c r="A366" s="106"/>
+      <c r="B366" s="106"/>
+      <c r="C366" s="106"/>
+      <c r="D366" s="106"/>
+      <c r="E366" s="106"/>
+      <c r="F366" s="106"/>
+      <c r="G366" s="106"/>
+      <c r="H366" s="106"/>
+      <c r="I366" s="106"/>
+      <c r="J366" s="106"/>
+      <c r="K366" s="106"/>
     </row>
     <row r="367" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A367" s="104" t="s">
+      <c r="A367" s="107" t="s">
         <v>275</v>
       </c>
-      <c r="B367" s="105"/>
-      <c r="C367" s="105"/>
-      <c r="D367" s="105"/>
-      <c r="E367" s="105"/>
-      <c r="F367" s="105"/>
-      <c r="G367" s="105"/>
-      <c r="H367" s="105"/>
-      <c r="I367" s="105"/>
-      <c r="J367" s="105"/>
-      <c r="K367" s="106"/>
+      <c r="B367" s="108"/>
+      <c r="C367" s="108"/>
+      <c r="D367" s="108"/>
+      <c r="E367" s="108"/>
+      <c r="F367" s="108"/>
+      <c r="G367" s="108"/>
+      <c r="H367" s="108"/>
+      <c r="I367" s="108"/>
+      <c r="J367" s="108"/>
+      <c r="K367" s="109"/>
     </row>
     <row r="368" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A368" s="20" t="s">
@@ -11345,7 +11369,7 @@
         <v>0</v>
       </c>
       <c r="F375" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G375" s="13" t="s">
         <v>11</v>
@@ -11360,45 +11384,45 @@
       </c>
     </row>
     <row r="376" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A376" s="107"/>
-      <c r="B376" s="107"/>
-      <c r="C376" s="107"/>
-      <c r="D376" s="107"/>
-      <c r="E376" s="107"/>
-      <c r="F376" s="107"/>
-      <c r="G376" s="107"/>
-      <c r="H376" s="107"/>
-      <c r="I376" s="107"/>
-      <c r="J376" s="107"/>
-      <c r="K376" s="107"/>
+      <c r="A376" s="110"/>
+      <c r="B376" s="110"/>
+      <c r="C376" s="110"/>
+      <c r="D376" s="110"/>
+      <c r="E376" s="110"/>
+      <c r="F376" s="110"/>
+      <c r="G376" s="110"/>
+      <c r="H376" s="110"/>
+      <c r="I376" s="110"/>
+      <c r="J376" s="110"/>
+      <c r="K376" s="110"/>
     </row>
     <row r="377" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A377" s="103"/>
-      <c r="B377" s="103"/>
-      <c r="C377" s="103"/>
-      <c r="D377" s="103"/>
-      <c r="E377" s="103"/>
-      <c r="F377" s="103"/>
-      <c r="G377" s="103"/>
-      <c r="H377" s="103"/>
-      <c r="I377" s="103"/>
-      <c r="J377" s="103"/>
-      <c r="K377" s="103"/>
+      <c r="A377" s="106"/>
+      <c r="B377" s="106"/>
+      <c r="C377" s="106"/>
+      <c r="D377" s="106"/>
+      <c r="E377" s="106"/>
+      <c r="F377" s="106"/>
+      <c r="G377" s="106"/>
+      <c r="H377" s="106"/>
+      <c r="I377" s="106"/>
+      <c r="J377" s="106"/>
+      <c r="K377" s="106"/>
     </row>
     <row r="378" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A378" s="104" t="s">
+      <c r="A378" s="107" t="s">
         <v>182</v>
       </c>
-      <c r="B378" s="105"/>
-      <c r="C378" s="105"/>
-      <c r="D378" s="105"/>
-      <c r="E378" s="105"/>
-      <c r="F378" s="105"/>
-      <c r="G378" s="105"/>
-      <c r="H378" s="105"/>
-      <c r="I378" s="105"/>
-      <c r="J378" s="105"/>
-      <c r="K378" s="106"/>
+      <c r="B378" s="108"/>
+      <c r="C378" s="108"/>
+      <c r="D378" s="108"/>
+      <c r="E378" s="108"/>
+      <c r="F378" s="108"/>
+      <c r="G378" s="108"/>
+      <c r="H378" s="108"/>
+      <c r="I378" s="108"/>
+      <c r="J378" s="108"/>
+      <c r="K378" s="109"/>
     </row>
     <row r="379" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A379" s="20" t="s">
@@ -11655,7 +11679,7 @@
         <v>0</v>
       </c>
       <c r="F387" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G387" s="13" t="s">
         <v>11</v>
@@ -11670,45 +11694,45 @@
       </c>
     </row>
     <row r="388" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A388" s="102"/>
-      <c r="B388" s="102"/>
-      <c r="C388" s="102"/>
-      <c r="D388" s="102"/>
-      <c r="E388" s="102"/>
-      <c r="F388" s="102"/>
-      <c r="G388" s="102"/>
-      <c r="H388" s="102"/>
-      <c r="I388" s="102"/>
-      <c r="J388" s="102"/>
-      <c r="K388" s="102"/>
+      <c r="A388" s="105"/>
+      <c r="B388" s="105"/>
+      <c r="C388" s="105"/>
+      <c r="D388" s="105"/>
+      <c r="E388" s="105"/>
+      <c r="F388" s="105"/>
+      <c r="G388" s="105"/>
+      <c r="H388" s="105"/>
+      <c r="I388" s="105"/>
+      <c r="J388" s="105"/>
+      <c r="K388" s="105"/>
     </row>
     <row r="389" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A389" s="103"/>
-      <c r="B389" s="103"/>
-      <c r="C389" s="103"/>
-      <c r="D389" s="103"/>
-      <c r="E389" s="103"/>
-      <c r="F389" s="103"/>
-      <c r="G389" s="103"/>
-      <c r="H389" s="103"/>
-      <c r="I389" s="103"/>
-      <c r="J389" s="103"/>
-      <c r="K389" s="103"/>
+      <c r="A389" s="106"/>
+      <c r="B389" s="106"/>
+      <c r="C389" s="106"/>
+      <c r="D389" s="106"/>
+      <c r="E389" s="106"/>
+      <c r="F389" s="106"/>
+      <c r="G389" s="106"/>
+      <c r="H389" s="106"/>
+      <c r="I389" s="106"/>
+      <c r="J389" s="106"/>
+      <c r="K389" s="106"/>
     </row>
     <row r="390" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A390" s="104" t="s">
+      <c r="A390" s="107" t="s">
         <v>256</v>
       </c>
-      <c r="B390" s="105"/>
-      <c r="C390" s="105"/>
-      <c r="D390" s="105"/>
-      <c r="E390" s="105"/>
-      <c r="F390" s="105"/>
-      <c r="G390" s="105"/>
-      <c r="H390" s="105"/>
-      <c r="I390" s="105"/>
-      <c r="J390" s="105"/>
-      <c r="K390" s="106"/>
+      <c r="B390" s="108"/>
+      <c r="C390" s="108"/>
+      <c r="D390" s="108"/>
+      <c r="E390" s="108"/>
+      <c r="F390" s="108"/>
+      <c r="G390" s="108"/>
+      <c r="H390" s="108"/>
+      <c r="I390" s="108"/>
+      <c r="J390" s="108"/>
+      <c r="K390" s="109"/>
     </row>
     <row r="391" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A391" s="20" t="s">
@@ -11903,7 +11927,7 @@
         <v>0</v>
       </c>
       <c r="F397" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G397" s="13" t="s">
         <v>11</v>
@@ -11918,45 +11942,45 @@
       </c>
     </row>
     <row r="398" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A398" s="102"/>
-      <c r="B398" s="102"/>
-      <c r="C398" s="102"/>
-      <c r="D398" s="102"/>
-      <c r="E398" s="102"/>
-      <c r="F398" s="102"/>
-      <c r="G398" s="102"/>
-      <c r="H398" s="102"/>
-      <c r="I398" s="102"/>
-      <c r="J398" s="102"/>
-      <c r="K398" s="102"/>
+      <c r="A398" s="105"/>
+      <c r="B398" s="105"/>
+      <c r="C398" s="105"/>
+      <c r="D398" s="105"/>
+      <c r="E398" s="105"/>
+      <c r="F398" s="105"/>
+      <c r="G398" s="105"/>
+      <c r="H398" s="105"/>
+      <c r="I398" s="105"/>
+      <c r="J398" s="105"/>
+      <c r="K398" s="105"/>
     </row>
     <row r="399" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A399" s="103"/>
-      <c r="B399" s="103"/>
-      <c r="C399" s="103"/>
-      <c r="D399" s="103"/>
-      <c r="E399" s="103"/>
-      <c r="F399" s="103"/>
-      <c r="G399" s="103"/>
-      <c r="H399" s="103"/>
-      <c r="I399" s="103"/>
-      <c r="J399" s="103"/>
-      <c r="K399" s="103"/>
+      <c r="A399" s="106"/>
+      <c r="B399" s="106"/>
+      <c r="C399" s="106"/>
+      <c r="D399" s="106"/>
+      <c r="E399" s="106"/>
+      <c r="F399" s="106"/>
+      <c r="G399" s="106"/>
+      <c r="H399" s="106"/>
+      <c r="I399" s="106"/>
+      <c r="J399" s="106"/>
+      <c r="K399" s="106"/>
     </row>
     <row r="400" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A400" s="104" t="s">
+      <c r="A400" s="107" t="s">
         <v>262</v>
       </c>
-      <c r="B400" s="105"/>
-      <c r="C400" s="105"/>
-      <c r="D400" s="105"/>
-      <c r="E400" s="105"/>
-      <c r="F400" s="105"/>
-      <c r="G400" s="105"/>
-      <c r="H400" s="105"/>
-      <c r="I400" s="105"/>
-      <c r="J400" s="105"/>
-      <c r="K400" s="106"/>
+      <c r="B400" s="108"/>
+      <c r="C400" s="108"/>
+      <c r="D400" s="108"/>
+      <c r="E400" s="108"/>
+      <c r="F400" s="108"/>
+      <c r="G400" s="108"/>
+      <c r="H400" s="108"/>
+      <c r="I400" s="108"/>
+      <c r="J400" s="108"/>
+      <c r="K400" s="109"/>
     </row>
     <row r="401" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A401" s="20" t="s">
@@ -12151,7 +12175,7 @@
         <v>0</v>
       </c>
       <c r="F407" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G407" s="13" t="s">
         <v>11</v>
@@ -12166,45 +12190,45 @@
       </c>
     </row>
     <row r="408" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A408" s="102"/>
-      <c r="B408" s="102"/>
-      <c r="C408" s="102"/>
-      <c r="D408" s="102"/>
-      <c r="E408" s="102"/>
-      <c r="F408" s="102"/>
-      <c r="G408" s="102"/>
-      <c r="H408" s="102"/>
-      <c r="I408" s="102"/>
-      <c r="J408" s="102"/>
-      <c r="K408" s="102"/>
+      <c r="A408" s="105"/>
+      <c r="B408" s="105"/>
+      <c r="C408" s="105"/>
+      <c r="D408" s="105"/>
+      <c r="E408" s="105"/>
+      <c r="F408" s="105"/>
+      <c r="G408" s="105"/>
+      <c r="H408" s="105"/>
+      <c r="I408" s="105"/>
+      <c r="J408" s="105"/>
+      <c r="K408" s="105"/>
     </row>
     <row r="409" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A409" s="103"/>
-      <c r="B409" s="103"/>
-      <c r="C409" s="103"/>
-      <c r="D409" s="103"/>
-      <c r="E409" s="103"/>
-      <c r="F409" s="103"/>
-      <c r="G409" s="103"/>
-      <c r="H409" s="103"/>
-      <c r="I409" s="103"/>
-      <c r="J409" s="103"/>
-      <c r="K409" s="103"/>
+      <c r="A409" s="106"/>
+      <c r="B409" s="106"/>
+      <c r="C409" s="106"/>
+      <c r="D409" s="106"/>
+      <c r="E409" s="106"/>
+      <c r="F409" s="106"/>
+      <c r="G409" s="106"/>
+      <c r="H409" s="106"/>
+      <c r="I409" s="106"/>
+      <c r="J409" s="106"/>
+      <c r="K409" s="106"/>
     </row>
     <row r="410" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A410" s="104" t="s">
+      <c r="A410" s="107" t="s">
         <v>265</v>
       </c>
-      <c r="B410" s="105"/>
-      <c r="C410" s="105"/>
-      <c r="D410" s="105"/>
-      <c r="E410" s="105"/>
-      <c r="F410" s="105"/>
-      <c r="G410" s="105"/>
-      <c r="H410" s="105"/>
-      <c r="I410" s="105"/>
-      <c r="J410" s="105"/>
-      <c r="K410" s="106"/>
+      <c r="B410" s="108"/>
+      <c r="C410" s="108"/>
+      <c r="D410" s="108"/>
+      <c r="E410" s="108"/>
+      <c r="F410" s="108"/>
+      <c r="G410" s="108"/>
+      <c r="H410" s="108"/>
+      <c r="I410" s="108"/>
+      <c r="J410" s="108"/>
+      <c r="K410" s="109"/>
     </row>
     <row r="411" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A411" s="20" t="s">
@@ -12393,7 +12417,7 @@
         <v>0</v>
       </c>
       <c r="F417" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G417" s="13" t="s">
         <v>11</v>
@@ -12408,45 +12432,45 @@
       </c>
     </row>
     <row r="418" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A418" s="102"/>
-      <c r="B418" s="102"/>
-      <c r="C418" s="102"/>
-      <c r="D418" s="102"/>
-      <c r="E418" s="102"/>
-      <c r="F418" s="102"/>
-      <c r="G418" s="102"/>
-      <c r="H418" s="102"/>
-      <c r="I418" s="102"/>
-      <c r="J418" s="102"/>
-      <c r="K418" s="102"/>
+      <c r="A418" s="105"/>
+      <c r="B418" s="105"/>
+      <c r="C418" s="105"/>
+      <c r="D418" s="105"/>
+      <c r="E418" s="105"/>
+      <c r="F418" s="105"/>
+      <c r="G418" s="105"/>
+      <c r="H418" s="105"/>
+      <c r="I418" s="105"/>
+      <c r="J418" s="105"/>
+      <c r="K418" s="105"/>
     </row>
     <row r="419" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A419" s="103"/>
-      <c r="B419" s="103"/>
-      <c r="C419" s="103"/>
-      <c r="D419" s="103"/>
-      <c r="E419" s="103"/>
-      <c r="F419" s="103"/>
-      <c r="G419" s="103"/>
-      <c r="H419" s="103"/>
-      <c r="I419" s="103"/>
-      <c r="J419" s="103"/>
-      <c r="K419" s="103"/>
+      <c r="A419" s="106"/>
+      <c r="B419" s="106"/>
+      <c r="C419" s="106"/>
+      <c r="D419" s="106"/>
+      <c r="E419" s="106"/>
+      <c r="F419" s="106"/>
+      <c r="G419" s="106"/>
+      <c r="H419" s="106"/>
+      <c r="I419" s="106"/>
+      <c r="J419" s="106"/>
+      <c r="K419" s="106"/>
     </row>
     <row r="420" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A420" s="104" t="s">
+      <c r="A420" s="107" t="s">
         <v>268</v>
       </c>
-      <c r="B420" s="105"/>
-      <c r="C420" s="105"/>
-      <c r="D420" s="105"/>
-      <c r="E420" s="105"/>
-      <c r="F420" s="105"/>
-      <c r="G420" s="105"/>
-      <c r="H420" s="105"/>
-      <c r="I420" s="105"/>
-      <c r="J420" s="105"/>
-      <c r="K420" s="106"/>
+      <c r="B420" s="108"/>
+      <c r="C420" s="108"/>
+      <c r="D420" s="108"/>
+      <c r="E420" s="108"/>
+      <c r="F420" s="108"/>
+      <c r="G420" s="108"/>
+      <c r="H420" s="108"/>
+      <c r="I420" s="108"/>
+      <c r="J420" s="108"/>
+      <c r="K420" s="109"/>
     </row>
     <row r="421" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A421" s="20" t="s">
@@ -12664,7 +12688,7 @@
         <v>0</v>
       </c>
       <c r="F428" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G428" s="13" t="s">
         <v>11</v>
@@ -12679,45 +12703,45 @@
       </c>
     </row>
     <row r="429" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A429" s="102"/>
-      <c r="B429" s="102"/>
-      <c r="C429" s="102"/>
-      <c r="D429" s="102"/>
-      <c r="E429" s="102"/>
-      <c r="F429" s="102"/>
-      <c r="G429" s="102"/>
-      <c r="H429" s="102"/>
-      <c r="I429" s="102"/>
-      <c r="J429" s="102"/>
-      <c r="K429" s="102"/>
+      <c r="A429" s="105"/>
+      <c r="B429" s="105"/>
+      <c r="C429" s="105"/>
+      <c r="D429" s="105"/>
+      <c r="E429" s="105"/>
+      <c r="F429" s="105"/>
+      <c r="G429" s="105"/>
+      <c r="H429" s="105"/>
+      <c r="I429" s="105"/>
+      <c r="J429" s="105"/>
+      <c r="K429" s="105"/>
     </row>
     <row r="430" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A430" s="103"/>
-      <c r="B430" s="103"/>
-      <c r="C430" s="103"/>
-      <c r="D430" s="103"/>
-      <c r="E430" s="103"/>
-      <c r="F430" s="103"/>
-      <c r="G430" s="103"/>
-      <c r="H430" s="103"/>
-      <c r="I430" s="103"/>
-      <c r="J430" s="103"/>
-      <c r="K430" s="103"/>
+      <c r="A430" s="106"/>
+      <c r="B430" s="106"/>
+      <c r="C430" s="106"/>
+      <c r="D430" s="106"/>
+      <c r="E430" s="106"/>
+      <c r="F430" s="106"/>
+      <c r="G430" s="106"/>
+      <c r="H430" s="106"/>
+      <c r="I430" s="106"/>
+      <c r="J430" s="106"/>
+      <c r="K430" s="106"/>
     </row>
     <row r="431" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A431" s="104" t="s">
+      <c r="A431" s="107" t="s">
         <v>271</v>
       </c>
-      <c r="B431" s="105"/>
-      <c r="C431" s="105"/>
-      <c r="D431" s="105"/>
-      <c r="E431" s="105"/>
-      <c r="F431" s="105"/>
-      <c r="G431" s="105"/>
-      <c r="H431" s="105"/>
-      <c r="I431" s="105"/>
-      <c r="J431" s="105"/>
-      <c r="K431" s="106"/>
+      <c r="B431" s="108"/>
+      <c r="C431" s="108"/>
+      <c r="D431" s="108"/>
+      <c r="E431" s="108"/>
+      <c r="F431" s="108"/>
+      <c r="G431" s="108"/>
+      <c r="H431" s="108"/>
+      <c r="I431" s="108"/>
+      <c r="J431" s="108"/>
+      <c r="K431" s="109"/>
     </row>
     <row r="432" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A432" s="20" t="s">
@@ -12882,7 +12906,7 @@
         <v>0</v>
       </c>
       <c r="F437" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G437" s="13" t="s">
         <v>11</v>
@@ -12897,45 +12921,45 @@
       </c>
     </row>
     <row r="438" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A438" s="102"/>
-      <c r="B438" s="102"/>
-      <c r="C438" s="102"/>
-      <c r="D438" s="102"/>
-      <c r="E438" s="102"/>
-      <c r="F438" s="102"/>
-      <c r="G438" s="102"/>
-      <c r="H438" s="102"/>
-      <c r="I438" s="102"/>
-      <c r="J438" s="102"/>
-      <c r="K438" s="102"/>
+      <c r="A438" s="105"/>
+      <c r="B438" s="105"/>
+      <c r="C438" s="105"/>
+      <c r="D438" s="105"/>
+      <c r="E438" s="105"/>
+      <c r="F438" s="105"/>
+      <c r="G438" s="105"/>
+      <c r="H438" s="105"/>
+      <c r="I438" s="105"/>
+      <c r="J438" s="105"/>
+      <c r="K438" s="105"/>
     </row>
     <row r="439" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A439" s="103"/>
-      <c r="B439" s="103"/>
-      <c r="C439" s="103"/>
-      <c r="D439" s="103"/>
-      <c r="E439" s="103"/>
-      <c r="F439" s="103"/>
-      <c r="G439" s="103"/>
-      <c r="H439" s="103"/>
-      <c r="I439" s="103"/>
-      <c r="J439" s="103"/>
-      <c r="K439" s="103"/>
+      <c r="A439" s="106"/>
+      <c r="B439" s="106"/>
+      <c r="C439" s="106"/>
+      <c r="D439" s="106"/>
+      <c r="E439" s="106"/>
+      <c r="F439" s="106"/>
+      <c r="G439" s="106"/>
+      <c r="H439" s="106"/>
+      <c r="I439" s="106"/>
+      <c r="J439" s="106"/>
+      <c r="K439" s="106"/>
     </row>
     <row r="440" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A440" s="104" t="s">
+      <c r="A440" s="107" t="s">
         <v>273</v>
       </c>
-      <c r="B440" s="105"/>
-      <c r="C440" s="105"/>
-      <c r="D440" s="105"/>
-      <c r="E440" s="105"/>
-      <c r="F440" s="105"/>
-      <c r="G440" s="105"/>
-      <c r="H440" s="105"/>
-      <c r="I440" s="105"/>
-      <c r="J440" s="105"/>
-      <c r="K440" s="106"/>
+      <c r="B440" s="108"/>
+      <c r="C440" s="108"/>
+      <c r="D440" s="108"/>
+      <c r="E440" s="108"/>
+      <c r="F440" s="108"/>
+      <c r="G440" s="108"/>
+      <c r="H440" s="108"/>
+      <c r="I440" s="108"/>
+      <c r="J440" s="108"/>
+      <c r="K440" s="109"/>
     </row>
     <row r="441" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A441" s="20" t="s">
@@ -13211,7 +13235,7 @@
         <v>0</v>
       </c>
       <c r="F450" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G450" s="13" t="s">
         <v>11</v>
@@ -13226,45 +13250,45 @@
       </c>
     </row>
     <row r="451" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A451" s="102"/>
-      <c r="B451" s="102"/>
-      <c r="C451" s="102"/>
-      <c r="D451" s="102"/>
-      <c r="E451" s="102"/>
-      <c r="F451" s="102"/>
-      <c r="G451" s="102"/>
-      <c r="H451" s="102"/>
-      <c r="I451" s="102"/>
-      <c r="J451" s="102"/>
-      <c r="K451" s="102"/>
+      <c r="A451" s="105"/>
+      <c r="B451" s="105"/>
+      <c r="C451" s="105"/>
+      <c r="D451" s="105"/>
+      <c r="E451" s="105"/>
+      <c r="F451" s="105"/>
+      <c r="G451" s="105"/>
+      <c r="H451" s="105"/>
+      <c r="I451" s="105"/>
+      <c r="J451" s="105"/>
+      <c r="K451" s="105"/>
     </row>
     <row r="452" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A452" s="103"/>
-      <c r="B452" s="103"/>
-      <c r="C452" s="103"/>
-      <c r="D452" s="103"/>
-      <c r="E452" s="103"/>
-      <c r="F452" s="103"/>
-      <c r="G452" s="103"/>
-      <c r="H452" s="103"/>
-      <c r="I452" s="103"/>
-      <c r="J452" s="103"/>
-      <c r="K452" s="103"/>
+      <c r="A452" s="106"/>
+      <c r="B452" s="106"/>
+      <c r="C452" s="106"/>
+      <c r="D452" s="106"/>
+      <c r="E452" s="106"/>
+      <c r="F452" s="106"/>
+      <c r="G452" s="106"/>
+      <c r="H452" s="106"/>
+      <c r="I452" s="106"/>
+      <c r="J452" s="106"/>
+      <c r="K452" s="106"/>
     </row>
     <row r="453" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A453" s="104" t="s">
+      <c r="A453" s="107" t="s">
         <v>285</v>
       </c>
-      <c r="B453" s="105"/>
-      <c r="C453" s="105"/>
-      <c r="D453" s="105"/>
-      <c r="E453" s="105"/>
-      <c r="F453" s="105"/>
-      <c r="G453" s="105"/>
-      <c r="H453" s="105"/>
-      <c r="I453" s="105"/>
-      <c r="J453" s="105"/>
-      <c r="K453" s="106"/>
+      <c r="B453" s="108"/>
+      <c r="C453" s="108"/>
+      <c r="D453" s="108"/>
+      <c r="E453" s="108"/>
+      <c r="F453" s="108"/>
+      <c r="G453" s="108"/>
+      <c r="H453" s="108"/>
+      <c r="I453" s="108"/>
+      <c r="J453" s="108"/>
+      <c r="K453" s="109"/>
     </row>
     <row r="454" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A454" s="20" t="s">
@@ -13523,7 +13547,7 @@
         <v>0</v>
       </c>
       <c r="F462" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G462" s="13" t="s">
         <v>11</v>
@@ -13537,8 +13561,262 @@
         <v>42</v>
       </c>
     </row>
+    <row r="463" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A463" s="105"/>
+      <c r="B463" s="105"/>
+      <c r="C463" s="105"/>
+      <c r="D463" s="105"/>
+      <c r="E463" s="105"/>
+      <c r="F463" s="105"/>
+      <c r="G463" s="105"/>
+      <c r="H463" s="105"/>
+      <c r="I463" s="105"/>
+      <c r="J463" s="105"/>
+      <c r="K463" s="105"/>
+    </row>
+    <row r="464" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A464" s="106"/>
+      <c r="B464" s="106"/>
+      <c r="C464" s="106"/>
+      <c r="D464" s="106"/>
+      <c r="E464" s="106"/>
+      <c r="F464" s="106"/>
+      <c r="G464" s="106"/>
+      <c r="H464" s="106"/>
+      <c r="I464" s="106"/>
+      <c r="J464" s="106"/>
+      <c r="K464" s="106"/>
+    </row>
+    <row r="465" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A465" s="107" t="s">
+        <v>304</v>
+      </c>
+      <c r="B465" s="108"/>
+      <c r="C465" s="108"/>
+      <c r="D465" s="108"/>
+      <c r="E465" s="108"/>
+      <c r="F465" s="108"/>
+      <c r="G465" s="108"/>
+      <c r="H465" s="108"/>
+      <c r="I465" s="108"/>
+      <c r="J465" s="108"/>
+      <c r="K465" s="109"/>
+    </row>
+    <row r="466" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A466" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B466" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C466" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D466" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="E466" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="F466" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="G466" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="H466" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="I466" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="J466" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="K466" s="19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="467" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A467" s="39">
+        <v>1</v>
+      </c>
+      <c r="B467" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C467" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="D467" s="5">
+        <v>20</v>
+      </c>
+      <c r="E467" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F467" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G467" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H467" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="I467" s="102" t="s">
+        <v>12</v>
+      </c>
+      <c r="J467" s="102"/>
+      <c r="K467" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="468" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A468" s="40">
+        <v>2</v>
+      </c>
+      <c r="B468" s="7" t="s">
+        <v>305</v>
+      </c>
+      <c r="C468" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D468" s="7">
+        <v>10</v>
+      </c>
+      <c r="E468" s="7"/>
+      <c r="F468" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G468" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H468" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="I468" s="104"/>
+      <c r="J468" s="104" t="s">
+        <v>12</v>
+      </c>
+      <c r="K468" s="9"/>
+    </row>
+    <row r="469" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A469" s="40">
+        <v>3</v>
+      </c>
+      <c r="B469" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="C469" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D469" s="7">
+        <v>10</v>
+      </c>
+      <c r="E469" s="7"/>
+      <c r="F469" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G469" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H469" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="I469" s="104"/>
+      <c r="J469" s="104" t="s">
+        <v>12</v>
+      </c>
+      <c r="K469" s="9"/>
+    </row>
+    <row r="470" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A470" s="40">
+        <v>4</v>
+      </c>
+      <c r="B470" s="7" t="s">
+        <v>307</v>
+      </c>
+      <c r="C470" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D470" s="7">
+        <v>1</v>
+      </c>
+      <c r="E470" s="7"/>
+      <c r="F470" s="7">
+        <v>3</v>
+      </c>
+      <c r="G470" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H470" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="I470" s="104"/>
+      <c r="J470" s="104" t="s">
+        <v>12</v>
+      </c>
+      <c r="K470" s="9" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="471" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A471" s="40">
+        <v>5</v>
+      </c>
+      <c r="B471" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C471" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D471" s="7"/>
+      <c r="E471" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F471" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G471" s="7"/>
+      <c r="H471" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="I471" s="104"/>
+      <c r="J471" s="104"/>
+      <c r="K471" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="472" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A472" s="41">
+        <v>6</v>
+      </c>
+      <c r="B472" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C472" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D472" s="13"/>
+      <c r="E472" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="F472" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="G472" s="13"/>
+      <c r="H472" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="I472" s="103"/>
+      <c r="J472" s="103"/>
+      <c r="K472" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="77">
+  <mergeCells count="79">
+    <mergeCell ref="A463:K464"/>
+    <mergeCell ref="A465:K465"/>
     <mergeCell ref="A451:K452"/>
     <mergeCell ref="A453:K453"/>
     <mergeCell ref="A1:K1"/>
@@ -13687,45 +13965,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="102"/>
-      <c r="B1" s="102"/>
-      <c r="C1" s="102"/>
-      <c r="D1" s="102"/>
-      <c r="E1" s="102"/>
-      <c r="F1" s="102"/>
-      <c r="G1" s="102"/>
-      <c r="H1" s="102"/>
-      <c r="I1" s="102"/>
-      <c r="J1" s="102"/>
-      <c r="K1" s="102"/>
+      <c r="A1" s="105"/>
+      <c r="B1" s="105"/>
+      <c r="C1" s="105"/>
+      <c r="D1" s="105"/>
+      <c r="E1" s="105"/>
+      <c r="F1" s="105"/>
+      <c r="G1" s="105"/>
+      <c r="H1" s="105"/>
+      <c r="I1" s="105"/>
+      <c r="J1" s="105"/>
+      <c r="K1" s="105"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="103"/>
-      <c r="B2" s="103"/>
-      <c r="C2" s="103"/>
-      <c r="D2" s="103"/>
-      <c r="E2" s="103"/>
-      <c r="F2" s="103"/>
-      <c r="G2" s="103"/>
-      <c r="H2" s="103"/>
-      <c r="I2" s="103"/>
-      <c r="J2" s="103"/>
-      <c r="K2" s="103"/>
+      <c r="A2" s="106"/>
+      <c r="B2" s="106"/>
+      <c r="C2" s="106"/>
+      <c r="D2" s="106"/>
+      <c r="E2" s="106"/>
+      <c r="F2" s="106"/>
+      <c r="G2" s="106"/>
+      <c r="H2" s="106"/>
+      <c r="I2" s="106"/>
+      <c r="J2" s="106"/>
+      <c r="K2" s="106"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="104" t="s">
+      <c r="A3" s="107" t="s">
         <v>99</v>
       </c>
-      <c r="B3" s="105"/>
-      <c r="C3" s="105"/>
-      <c r="D3" s="105"/>
-      <c r="E3" s="105"/>
-      <c r="F3" s="105"/>
-      <c r="G3" s="105"/>
-      <c r="H3" s="105"/>
-      <c r="I3" s="105"/>
-      <c r="J3" s="105"/>
-      <c r="K3" s="106"/>
+      <c r="B3" s="108"/>
+      <c r="C3" s="108"/>
+      <c r="D3" s="108"/>
+      <c r="E3" s="108"/>
+      <c r="F3" s="108"/>
+      <c r="G3" s="108"/>
+      <c r="H3" s="108"/>
+      <c r="I3" s="108"/>
+      <c r="J3" s="108"/>
+      <c r="K3" s="109"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -13910,45 +14188,45 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="102"/>
-      <c r="B10" s="102"/>
-      <c r="C10" s="102"/>
-      <c r="D10" s="102"/>
-      <c r="E10" s="102"/>
-      <c r="F10" s="102"/>
-      <c r="G10" s="102"/>
-      <c r="H10" s="102"/>
-      <c r="I10" s="102"/>
-      <c r="J10" s="102"/>
-      <c r="K10" s="102"/>
+      <c r="A10" s="105"/>
+      <c r="B10" s="105"/>
+      <c r="C10" s="105"/>
+      <c r="D10" s="105"/>
+      <c r="E10" s="105"/>
+      <c r="F10" s="105"/>
+      <c r="G10" s="105"/>
+      <c r="H10" s="105"/>
+      <c r="I10" s="105"/>
+      <c r="J10" s="105"/>
+      <c r="K10" s="105"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="103"/>
-      <c r="B11" s="103"/>
-      <c r="C11" s="103"/>
-      <c r="D11" s="103"/>
-      <c r="E11" s="103"/>
-      <c r="F11" s="103"/>
-      <c r="G11" s="103"/>
-      <c r="H11" s="103"/>
-      <c r="I11" s="103"/>
-      <c r="J11" s="103"/>
-      <c r="K11" s="103"/>
+      <c r="A11" s="106"/>
+      <c r="B11" s="106"/>
+      <c r="C11" s="106"/>
+      <c r="D11" s="106"/>
+      <c r="E11" s="106"/>
+      <c r="F11" s="106"/>
+      <c r="G11" s="106"/>
+      <c r="H11" s="106"/>
+      <c r="I11" s="106"/>
+      <c r="J11" s="106"/>
+      <c r="K11" s="106"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="104" t="s">
+      <c r="A12" s="107" t="s">
         <v>95</v>
       </c>
-      <c r="B12" s="105"/>
-      <c r="C12" s="105"/>
-      <c r="D12" s="105"/>
-      <c r="E12" s="105"/>
-      <c r="F12" s="105"/>
-      <c r="G12" s="105"/>
-      <c r="H12" s="105"/>
-      <c r="I12" s="105"/>
-      <c r="J12" s="105"/>
-      <c r="K12" s="106"/>
+      <c r="B12" s="108"/>
+      <c r="C12" s="108"/>
+      <c r="D12" s="108"/>
+      <c r="E12" s="108"/>
+      <c r="F12" s="108"/>
+      <c r="G12" s="108"/>
+      <c r="H12" s="108"/>
+      <c r="I12" s="108"/>
+      <c r="J12" s="108"/>
+      <c r="K12" s="109"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
@@ -14220,45 +14498,45 @@
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="102"/>
-      <c r="B22" s="102"/>
-      <c r="C22" s="102"/>
-      <c r="D22" s="102"/>
-      <c r="E22" s="102"/>
-      <c r="F22" s="102"/>
-      <c r="G22" s="102"/>
-      <c r="H22" s="102"/>
-      <c r="I22" s="102"/>
-      <c r="J22" s="102"/>
-      <c r="K22" s="102"/>
+      <c r="A22" s="105"/>
+      <c r="B22" s="105"/>
+      <c r="C22" s="105"/>
+      <c r="D22" s="105"/>
+      <c r="E22" s="105"/>
+      <c r="F22" s="105"/>
+      <c r="G22" s="105"/>
+      <c r="H22" s="105"/>
+      <c r="I22" s="105"/>
+      <c r="J22" s="105"/>
+      <c r="K22" s="105"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="103"/>
-      <c r="B23" s="103"/>
-      <c r="C23" s="103"/>
-      <c r="D23" s="103"/>
-      <c r="E23" s="103"/>
-      <c r="F23" s="103"/>
-      <c r="G23" s="103"/>
-      <c r="H23" s="103"/>
-      <c r="I23" s="103"/>
-      <c r="J23" s="103"/>
-      <c r="K23" s="103"/>
+      <c r="A23" s="106"/>
+      <c r="B23" s="106"/>
+      <c r="C23" s="106"/>
+      <c r="D23" s="106"/>
+      <c r="E23" s="106"/>
+      <c r="F23" s="106"/>
+      <c r="G23" s="106"/>
+      <c r="H23" s="106"/>
+      <c r="I23" s="106"/>
+      <c r="J23" s="106"/>
+      <c r="K23" s="106"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="104" t="s">
+      <c r="A24" s="107" t="s">
         <v>101</v>
       </c>
-      <c r="B24" s="105"/>
-      <c r="C24" s="105"/>
-      <c r="D24" s="105"/>
-      <c r="E24" s="105"/>
-      <c r="F24" s="105"/>
-      <c r="G24" s="105"/>
-      <c r="H24" s="105"/>
-      <c r="I24" s="105"/>
-      <c r="J24" s="105"/>
-      <c r="K24" s="106"/>
+      <c r="B24" s="108"/>
+      <c r="C24" s="108"/>
+      <c r="D24" s="108"/>
+      <c r="E24" s="108"/>
+      <c r="F24" s="108"/>
+      <c r="G24" s="108"/>
+      <c r="H24" s="108"/>
+      <c r="I24" s="108"/>
+      <c r="J24" s="108"/>
+      <c r="K24" s="109"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
@@ -14505,45 +14783,45 @@
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="102"/>
-      <c r="B33" s="102"/>
-      <c r="C33" s="102"/>
-      <c r="D33" s="102"/>
-      <c r="E33" s="102"/>
-      <c r="F33" s="102"/>
-      <c r="G33" s="102"/>
-      <c r="H33" s="102"/>
-      <c r="I33" s="102"/>
-      <c r="J33" s="102"/>
-      <c r="K33" s="102"/>
+      <c r="A33" s="105"/>
+      <c r="B33" s="105"/>
+      <c r="C33" s="105"/>
+      <c r="D33" s="105"/>
+      <c r="E33" s="105"/>
+      <c r="F33" s="105"/>
+      <c r="G33" s="105"/>
+      <c r="H33" s="105"/>
+      <c r="I33" s="105"/>
+      <c r="J33" s="105"/>
+      <c r="K33" s="105"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="103"/>
-      <c r="B34" s="103"/>
-      <c r="C34" s="103"/>
-      <c r="D34" s="103"/>
-      <c r="E34" s="103"/>
-      <c r="F34" s="103"/>
-      <c r="G34" s="103"/>
-      <c r="H34" s="103"/>
-      <c r="I34" s="103"/>
-      <c r="J34" s="103"/>
-      <c r="K34" s="103"/>
+      <c r="A34" s="106"/>
+      <c r="B34" s="106"/>
+      <c r="C34" s="106"/>
+      <c r="D34" s="106"/>
+      <c r="E34" s="106"/>
+      <c r="F34" s="106"/>
+      <c r="G34" s="106"/>
+      <c r="H34" s="106"/>
+      <c r="I34" s="106"/>
+      <c r="J34" s="106"/>
+      <c r="K34" s="106"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="104" t="s">
+      <c r="A35" s="107" t="s">
         <v>107</v>
       </c>
-      <c r="B35" s="105"/>
-      <c r="C35" s="105"/>
-      <c r="D35" s="105"/>
-      <c r="E35" s="105"/>
-      <c r="F35" s="105"/>
-      <c r="G35" s="105"/>
-      <c r="H35" s="105"/>
-      <c r="I35" s="105"/>
-      <c r="J35" s="105"/>
-      <c r="K35" s="106"/>
+      <c r="B35" s="108"/>
+      <c r="C35" s="108"/>
+      <c r="D35" s="108"/>
+      <c r="E35" s="108"/>
+      <c r="F35" s="108"/>
+      <c r="G35" s="108"/>
+      <c r="H35" s="108"/>
+      <c r="I35" s="108"/>
+      <c r="J35" s="108"/>
+      <c r="K35" s="109"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
@@ -14817,45 +15095,45 @@
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="102"/>
-      <c r="B45" s="102"/>
-      <c r="C45" s="102"/>
-      <c r="D45" s="102"/>
-      <c r="E45" s="102"/>
-      <c r="F45" s="102"/>
-      <c r="G45" s="102"/>
-      <c r="H45" s="102"/>
-      <c r="I45" s="102"/>
-      <c r="J45" s="102"/>
-      <c r="K45" s="102"/>
+      <c r="A45" s="105"/>
+      <c r="B45" s="105"/>
+      <c r="C45" s="105"/>
+      <c r="D45" s="105"/>
+      <c r="E45" s="105"/>
+      <c r="F45" s="105"/>
+      <c r="G45" s="105"/>
+      <c r="H45" s="105"/>
+      <c r="I45" s="105"/>
+      <c r="J45" s="105"/>
+      <c r="K45" s="105"/>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="103"/>
-      <c r="B46" s="103"/>
-      <c r="C46" s="103"/>
-      <c r="D46" s="103"/>
-      <c r="E46" s="103"/>
-      <c r="F46" s="103"/>
-      <c r="G46" s="103"/>
-      <c r="H46" s="103"/>
-      <c r="I46" s="103"/>
-      <c r="J46" s="103"/>
-      <c r="K46" s="103"/>
+      <c r="A46" s="106"/>
+      <c r="B46" s="106"/>
+      <c r="C46" s="106"/>
+      <c r="D46" s="106"/>
+      <c r="E46" s="106"/>
+      <c r="F46" s="106"/>
+      <c r="G46" s="106"/>
+      <c r="H46" s="106"/>
+      <c r="I46" s="106"/>
+      <c r="J46" s="106"/>
+      <c r="K46" s="106"/>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" s="104" t="s">
+      <c r="A47" s="107" t="s">
         <v>112</v>
       </c>
-      <c r="B47" s="105"/>
-      <c r="C47" s="105"/>
-      <c r="D47" s="105"/>
-      <c r="E47" s="105"/>
-      <c r="F47" s="105"/>
-      <c r="G47" s="105"/>
-      <c r="H47" s="105"/>
-      <c r="I47" s="105"/>
-      <c r="J47" s="105"/>
-      <c r="K47" s="106"/>
+      <c r="B47" s="108"/>
+      <c r="C47" s="108"/>
+      <c r="D47" s="108"/>
+      <c r="E47" s="108"/>
+      <c r="F47" s="108"/>
+      <c r="G47" s="108"/>
+      <c r="H47" s="108"/>
+      <c r="I47" s="108"/>
+      <c r="J47" s="108"/>
+      <c r="K47" s="109"/>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
@@ -15098,45 +15376,45 @@
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A56" s="102"/>
-      <c r="B56" s="102"/>
-      <c r="C56" s="102"/>
-      <c r="D56" s="102"/>
-      <c r="E56" s="102"/>
-      <c r="F56" s="102"/>
-      <c r="G56" s="102"/>
-      <c r="H56" s="102"/>
-      <c r="I56" s="102"/>
-      <c r="J56" s="102"/>
-      <c r="K56" s="102"/>
+      <c r="A56" s="105"/>
+      <c r="B56" s="105"/>
+      <c r="C56" s="105"/>
+      <c r="D56" s="105"/>
+      <c r="E56" s="105"/>
+      <c r="F56" s="105"/>
+      <c r="G56" s="105"/>
+      <c r="H56" s="105"/>
+      <c r="I56" s="105"/>
+      <c r="J56" s="105"/>
+      <c r="K56" s="105"/>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A57" s="103"/>
-      <c r="B57" s="103"/>
-      <c r="C57" s="103"/>
-      <c r="D57" s="103"/>
-      <c r="E57" s="103"/>
-      <c r="F57" s="103"/>
-      <c r="G57" s="103"/>
-      <c r="H57" s="103"/>
-      <c r="I57" s="103"/>
-      <c r="J57" s="103"/>
-      <c r="K57" s="103"/>
+      <c r="A57" s="106"/>
+      <c r="B57" s="106"/>
+      <c r="C57" s="106"/>
+      <c r="D57" s="106"/>
+      <c r="E57" s="106"/>
+      <c r="F57" s="106"/>
+      <c r="G57" s="106"/>
+      <c r="H57" s="106"/>
+      <c r="I57" s="106"/>
+      <c r="J57" s="106"/>
+      <c r="K57" s="106"/>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A58" s="104" t="s">
+      <c r="A58" s="107" t="s">
         <v>117</v>
       </c>
-      <c r="B58" s="105"/>
-      <c r="C58" s="105"/>
-      <c r="D58" s="105"/>
-      <c r="E58" s="105"/>
-      <c r="F58" s="105"/>
-      <c r="G58" s="105"/>
-      <c r="H58" s="105"/>
-      <c r="I58" s="105"/>
-      <c r="J58" s="105"/>
-      <c r="K58" s="106"/>
+      <c r="B58" s="108"/>
+      <c r="C58" s="108"/>
+      <c r="D58" s="108"/>
+      <c r="E58" s="108"/>
+      <c r="F58" s="108"/>
+      <c r="G58" s="108"/>
+      <c r="H58" s="108"/>
+      <c r="I58" s="108"/>
+      <c r="J58" s="108"/>
+      <c r="K58" s="109"/>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
@@ -15379,45 +15657,45 @@
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A67" s="102"/>
-      <c r="B67" s="102"/>
-      <c r="C67" s="102"/>
-      <c r="D67" s="102"/>
-      <c r="E67" s="102"/>
-      <c r="F67" s="102"/>
-      <c r="G67" s="102"/>
-      <c r="H67" s="102"/>
-      <c r="I67" s="102"/>
-      <c r="J67" s="102"/>
-      <c r="K67" s="102"/>
+      <c r="A67" s="105"/>
+      <c r="B67" s="105"/>
+      <c r="C67" s="105"/>
+      <c r="D67" s="105"/>
+      <c r="E67" s="105"/>
+      <c r="F67" s="105"/>
+      <c r="G67" s="105"/>
+      <c r="H67" s="105"/>
+      <c r="I67" s="105"/>
+      <c r="J67" s="105"/>
+      <c r="K67" s="105"/>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A68" s="103"/>
-      <c r="B68" s="103"/>
-      <c r="C68" s="103"/>
-      <c r="D68" s="103"/>
-      <c r="E68" s="103"/>
-      <c r="F68" s="103"/>
-      <c r="G68" s="103"/>
-      <c r="H68" s="103"/>
-      <c r="I68" s="103"/>
-      <c r="J68" s="103"/>
-      <c r="K68" s="103"/>
+      <c r="A68" s="106"/>
+      <c r="B68" s="106"/>
+      <c r="C68" s="106"/>
+      <c r="D68" s="106"/>
+      <c r="E68" s="106"/>
+      <c r="F68" s="106"/>
+      <c r="G68" s="106"/>
+      <c r="H68" s="106"/>
+      <c r="I68" s="106"/>
+      <c r="J68" s="106"/>
+      <c r="K68" s="106"/>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A69" s="104" t="s">
+      <c r="A69" s="107" t="s">
         <v>85</v>
       </c>
-      <c r="B69" s="105"/>
-      <c r="C69" s="105"/>
-      <c r="D69" s="105"/>
-      <c r="E69" s="105"/>
-      <c r="F69" s="105"/>
-      <c r="G69" s="105"/>
-      <c r="H69" s="105"/>
-      <c r="I69" s="105"/>
-      <c r="J69" s="105"/>
-      <c r="K69" s="106"/>
+      <c r="B69" s="108"/>
+      <c r="C69" s="108"/>
+      <c r="D69" s="108"/>
+      <c r="E69" s="108"/>
+      <c r="F69" s="108"/>
+      <c r="G69" s="108"/>
+      <c r="H69" s="108"/>
+      <c r="I69" s="108"/>
+      <c r="J69" s="108"/>
+      <c r="K69" s="109"/>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
@@ -15741,45 +16019,45 @@
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A82" s="102"/>
-      <c r="B82" s="102"/>
-      <c r="C82" s="102"/>
-      <c r="D82" s="102"/>
-      <c r="E82" s="102"/>
-      <c r="F82" s="102"/>
-      <c r="G82" s="102"/>
-      <c r="H82" s="102"/>
-      <c r="I82" s="102"/>
-      <c r="J82" s="102"/>
-      <c r="K82" s="102"/>
+      <c r="A82" s="105"/>
+      <c r="B82" s="105"/>
+      <c r="C82" s="105"/>
+      <c r="D82" s="105"/>
+      <c r="E82" s="105"/>
+      <c r="F82" s="105"/>
+      <c r="G82" s="105"/>
+      <c r="H82" s="105"/>
+      <c r="I82" s="105"/>
+      <c r="J82" s="105"/>
+      <c r="K82" s="105"/>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A83" s="103"/>
-      <c r="B83" s="103"/>
-      <c r="C83" s="103"/>
-      <c r="D83" s="103"/>
-      <c r="E83" s="103"/>
-      <c r="F83" s="103"/>
-      <c r="G83" s="103"/>
-      <c r="H83" s="103"/>
-      <c r="I83" s="103"/>
-      <c r="J83" s="103"/>
-      <c r="K83" s="103"/>
+      <c r="A83" s="106"/>
+      <c r="B83" s="106"/>
+      <c r="C83" s="106"/>
+      <c r="D83" s="106"/>
+      <c r="E83" s="106"/>
+      <c r="F83" s="106"/>
+      <c r="G83" s="106"/>
+      <c r="H83" s="106"/>
+      <c r="I83" s="106"/>
+      <c r="J83" s="106"/>
+      <c r="K83" s="106"/>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A84" s="104" t="s">
+      <c r="A84" s="107" t="s">
         <v>192</v>
       </c>
-      <c r="B84" s="105"/>
-      <c r="C84" s="105"/>
-      <c r="D84" s="105"/>
-      <c r="E84" s="105"/>
-      <c r="F84" s="105"/>
-      <c r="G84" s="105"/>
-      <c r="H84" s="105"/>
-      <c r="I84" s="105"/>
-      <c r="J84" s="105"/>
-      <c r="K84" s="106"/>
+      <c r="B84" s="108"/>
+      <c r="C84" s="108"/>
+      <c r="D84" s="108"/>
+      <c r="E84" s="108"/>
+      <c r="F84" s="108"/>
+      <c r="G84" s="108"/>
+      <c r="H84" s="108"/>
+      <c r="I84" s="108"/>
+      <c r="J84" s="108"/>
+      <c r="K84" s="109"/>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="20" t="s">
@@ -15960,45 +16238,45 @@
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A91" s="102"/>
-      <c r="B91" s="102"/>
-      <c r="C91" s="102"/>
-      <c r="D91" s="102"/>
-      <c r="E91" s="102"/>
-      <c r="F91" s="102"/>
-      <c r="G91" s="102"/>
-      <c r="H91" s="102"/>
-      <c r="I91" s="102"/>
-      <c r="J91" s="102"/>
-      <c r="K91" s="102"/>
+      <c r="A91" s="105"/>
+      <c r="B91" s="105"/>
+      <c r="C91" s="105"/>
+      <c r="D91" s="105"/>
+      <c r="E91" s="105"/>
+      <c r="F91" s="105"/>
+      <c r="G91" s="105"/>
+      <c r="H91" s="105"/>
+      <c r="I91" s="105"/>
+      <c r="J91" s="105"/>
+      <c r="K91" s="105"/>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A92" s="103"/>
-      <c r="B92" s="103"/>
-      <c r="C92" s="103"/>
-      <c r="D92" s="103"/>
-      <c r="E92" s="103"/>
-      <c r="F92" s="103"/>
-      <c r="G92" s="103"/>
-      <c r="H92" s="103"/>
-      <c r="I92" s="103"/>
-      <c r="J92" s="103"/>
-      <c r="K92" s="103"/>
+      <c r="A92" s="106"/>
+      <c r="B92" s="106"/>
+      <c r="C92" s="106"/>
+      <c r="D92" s="106"/>
+      <c r="E92" s="106"/>
+      <c r="F92" s="106"/>
+      <c r="G92" s="106"/>
+      <c r="H92" s="106"/>
+      <c r="I92" s="106"/>
+      <c r="J92" s="106"/>
+      <c r="K92" s="106"/>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A93" s="104" t="s">
+      <c r="A93" s="107" t="s">
         <v>191</v>
       </c>
-      <c r="B93" s="105"/>
-      <c r="C93" s="105"/>
-      <c r="D93" s="105"/>
-      <c r="E93" s="105"/>
-      <c r="F93" s="105"/>
-      <c r="G93" s="105"/>
-      <c r="H93" s="105"/>
-      <c r="I93" s="105"/>
-      <c r="J93" s="105"/>
-      <c r="K93" s="106"/>
+      <c r="B93" s="108"/>
+      <c r="C93" s="108"/>
+      <c r="D93" s="108"/>
+      <c r="E93" s="108"/>
+      <c r="F93" s="108"/>
+      <c r="G93" s="108"/>
+      <c r="H93" s="108"/>
+      <c r="I93" s="108"/>
+      <c r="J93" s="108"/>
+      <c r="K93" s="109"/>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
@@ -16245,45 +16523,45 @@
       </c>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A103" s="102"/>
-      <c r="B103" s="102"/>
-      <c r="C103" s="102"/>
-      <c r="D103" s="102"/>
-      <c r="E103" s="102"/>
-      <c r="F103" s="102"/>
-      <c r="G103" s="102"/>
-      <c r="H103" s="102"/>
-      <c r="I103" s="102"/>
-      <c r="J103" s="102"/>
-      <c r="K103" s="102"/>
+      <c r="A103" s="105"/>
+      <c r="B103" s="105"/>
+      <c r="C103" s="105"/>
+      <c r="D103" s="105"/>
+      <c r="E103" s="105"/>
+      <c r="F103" s="105"/>
+      <c r="G103" s="105"/>
+      <c r="H103" s="105"/>
+      <c r="I103" s="105"/>
+      <c r="J103" s="105"/>
+      <c r="K103" s="105"/>
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A104" s="103"/>
-      <c r="B104" s="103"/>
-      <c r="C104" s="103"/>
-      <c r="D104" s="103"/>
-      <c r="E104" s="103"/>
-      <c r="F104" s="103"/>
-      <c r="G104" s="103"/>
-      <c r="H104" s="103"/>
-      <c r="I104" s="103"/>
-      <c r="J104" s="103"/>
-      <c r="K104" s="103"/>
+      <c r="A104" s="106"/>
+      <c r="B104" s="106"/>
+      <c r="C104" s="106"/>
+      <c r="D104" s="106"/>
+      <c r="E104" s="106"/>
+      <c r="F104" s="106"/>
+      <c r="G104" s="106"/>
+      <c r="H104" s="106"/>
+      <c r="I104" s="106"/>
+      <c r="J104" s="106"/>
+      <c r="K104" s="106"/>
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A105" s="104" t="s">
+      <c r="A105" s="107" t="s">
         <v>71</v>
       </c>
-      <c r="B105" s="105"/>
-      <c r="C105" s="105"/>
-      <c r="D105" s="105"/>
-      <c r="E105" s="105"/>
-      <c r="F105" s="105"/>
-      <c r="G105" s="105"/>
-      <c r="H105" s="105"/>
-      <c r="I105" s="105"/>
-      <c r="J105" s="105"/>
-      <c r="K105" s="106"/>
+      <c r="B105" s="108"/>
+      <c r="C105" s="108"/>
+      <c r="D105" s="108"/>
+      <c r="E105" s="108"/>
+      <c r="F105" s="108"/>
+      <c r="G105" s="108"/>
+      <c r="H105" s="108"/>
+      <c r="I105" s="108"/>
+      <c r="J105" s="108"/>
+      <c r="K105" s="109"/>
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" s="20" t="s">
@@ -16414,45 +16692,45 @@
       <c r="K109" s="14"/>
     </row>
     <row r="110" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A110" s="102"/>
-      <c r="B110" s="102"/>
-      <c r="C110" s="102"/>
-      <c r="D110" s="102"/>
-      <c r="E110" s="102"/>
-      <c r="F110" s="102"/>
-      <c r="G110" s="102"/>
-      <c r="H110" s="102"/>
-      <c r="I110" s="102"/>
-      <c r="J110" s="102"/>
-      <c r="K110" s="102"/>
+      <c r="A110" s="105"/>
+      <c r="B110" s="105"/>
+      <c r="C110" s="105"/>
+      <c r="D110" s="105"/>
+      <c r="E110" s="105"/>
+      <c r="F110" s="105"/>
+      <c r="G110" s="105"/>
+      <c r="H110" s="105"/>
+      <c r="I110" s="105"/>
+      <c r="J110" s="105"/>
+      <c r="K110" s="105"/>
     </row>
     <row r="111" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A111" s="103"/>
-      <c r="B111" s="103"/>
-      <c r="C111" s="103"/>
-      <c r="D111" s="103"/>
-      <c r="E111" s="103"/>
-      <c r="F111" s="103"/>
-      <c r="G111" s="103"/>
-      <c r="H111" s="103"/>
-      <c r="I111" s="103"/>
-      <c r="J111" s="103"/>
-      <c r="K111" s="103"/>
+      <c r="A111" s="106"/>
+      <c r="B111" s="106"/>
+      <c r="C111" s="106"/>
+      <c r="D111" s="106"/>
+      <c r="E111" s="106"/>
+      <c r="F111" s="106"/>
+      <c r="G111" s="106"/>
+      <c r="H111" s="106"/>
+      <c r="I111" s="106"/>
+      <c r="J111" s="106"/>
+      <c r="K111" s="106"/>
     </row>
     <row r="112" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A112" s="104" t="s">
+      <c r="A112" s="107" t="s">
         <v>73</v>
       </c>
-      <c r="B112" s="105"/>
-      <c r="C112" s="105"/>
-      <c r="D112" s="105"/>
-      <c r="E112" s="105"/>
-      <c r="F112" s="105"/>
-      <c r="G112" s="105"/>
-      <c r="H112" s="105"/>
-      <c r="I112" s="105"/>
-      <c r="J112" s="105"/>
-      <c r="K112" s="106"/>
+      <c r="B112" s="108"/>
+      <c r="C112" s="108"/>
+      <c r="D112" s="108"/>
+      <c r="E112" s="108"/>
+      <c r="F112" s="108"/>
+      <c r="G112" s="108"/>
+      <c r="H112" s="108"/>
+      <c r="I112" s="108"/>
+      <c r="J112" s="108"/>
+      <c r="K112" s="109"/>
     </row>
     <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113" s="20" t="s">

</xml_diff>